<commit_message>
rename and add data
</commit_message>
<xml_diff>
--- a/raw_data/Hypophysenpatienten.xlsx
+++ b/raw_data/Hypophysenpatienten.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27004"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27021"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tristan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D30FE6AF-F198-48FA-8DFC-EA61064E722E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F007C722-5E58-4DF3-BA96-42AE98AF9939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="w duplicates" sheetId="1" r:id="rId1"/>
     <sheet name="no duplicate PID" sheetId="3" r:id="rId2"/>
+    <sheet name="Mapping" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20236" uniqueCount="2498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20893" uniqueCount="2633">
   <si>
     <t>%ID</t>
   </si>
@@ -7506,21 +7507,18 @@
     <t xml:space="preserve">morbus cushing, cortico, </t>
   </si>
   <si>
+    <t>hyperprolakin stressinduziert</t>
+  </si>
+  <si>
     <t>kein mikroadenom</t>
   </si>
   <si>
-    <t>hyperprolakin stressinduziert</t>
-  </si>
-  <si>
     <t xml:space="preserve">hyperprolaktin stressbedingt, </t>
   </si>
   <si>
     <t>gondao, thyreo, cortico, SIADH</t>
   </si>
   <si>
-    <t>inaktiv (gonado), apoplex</t>
-  </si>
-  <si>
     <t>apoplex, DD: rathke oder kraniopharyngeom</t>
   </si>
   <si>
@@ -7531,6 +7529,414 @@
   </si>
   <si>
     <t>hyperprolaktin, hypogonado, hypothyreo</t>
+  </si>
+  <si>
+    <t>hyperprolaktin, hypogonado</t>
+  </si>
+  <si>
+    <t>hyperprolaktin, hypogonad</t>
+  </si>
+  <si>
+    <t>giant</t>
+  </si>
+  <si>
+    <t>chiasma, thyreo, gonado</t>
+  </si>
+  <si>
+    <t>inaktives, apoplektiformes gondaotropes hypophysen giant adenom</t>
+  </si>
+  <si>
+    <t>kein Adenom, Rathke Zyste</t>
+  </si>
+  <si>
+    <t>inaktiv, somatotrop</t>
+  </si>
+  <si>
+    <t>whrsch. kein Adenom</t>
+  </si>
+  <si>
+    <t>Rathkezyste</t>
+  </si>
+  <si>
+    <t>Kind</t>
+  </si>
+  <si>
+    <t>supprimiertes prolaktin</t>
+  </si>
+  <si>
+    <t>somato, thyreo, cortico</t>
+  </si>
+  <si>
+    <t>keine weiteren Angaben</t>
+  </si>
+  <si>
+    <t>thyreo, cortico</t>
+  </si>
+  <si>
+    <t>inakiv</t>
+  </si>
+  <si>
+    <t>inaktiv, rathke</t>
+  </si>
+  <si>
+    <t>somato, gonado</t>
+  </si>
+  <si>
+    <t>Vd.a. Mirkoadenom</t>
+  </si>
+  <si>
+    <t>kein Adenom, proteinreiche Rathke</t>
+  </si>
+  <si>
+    <t>prolaktin</t>
+  </si>
+  <si>
+    <t>inaktiv, supprimiert</t>
+  </si>
+  <si>
+    <t>prolaktin, gonado</t>
+  </si>
+  <si>
+    <t>269ug/l</t>
+  </si>
+  <si>
+    <t>22.7nmol</t>
+  </si>
+  <si>
+    <t>7ug/l</t>
+  </si>
+  <si>
+    <t>32.5nmol/l</t>
+  </si>
+  <si>
+    <t>38ug/l</t>
+  </si>
+  <si>
+    <t>13.5ug/L</t>
+  </si>
+  <si>
+    <t>16.6nmol</t>
+  </si>
+  <si>
+    <t>cortico, thyreo, ADH</t>
+  </si>
+  <si>
+    <t>extern Diamon</t>
+  </si>
+  <si>
+    <t>52.8ug/l</t>
+  </si>
+  <si>
+    <t>normalbefund</t>
+  </si>
+  <si>
+    <t>80ug/l</t>
+  </si>
+  <si>
+    <t>77.7nmol</t>
+  </si>
+  <si>
+    <t>381ug/l</t>
+  </si>
+  <si>
+    <t>15.9nmol</t>
+  </si>
+  <si>
+    <t>Testo 3.8nmol</t>
+  </si>
+  <si>
+    <t>366ug/l</t>
+  </si>
+  <si>
+    <t>14.9nmol</t>
+  </si>
+  <si>
+    <t>FSH 0.4U/L</t>
+  </si>
+  <si>
+    <t>9.9ug/l</t>
+  </si>
+  <si>
+    <t>Testo 1.7nmol</t>
+  </si>
+  <si>
+    <t>954ug/l</t>
+  </si>
+  <si>
+    <t>22nmol</t>
+  </si>
+  <si>
+    <t>FSH 0.7U/L</t>
+  </si>
+  <si>
+    <t>gonado, somato, cortico</t>
+  </si>
+  <si>
+    <t>2.7ug/l</t>
+  </si>
+  <si>
+    <t>Testo 5.7</t>
+  </si>
+  <si>
+    <t>thyreo, cortico, somato</t>
+  </si>
+  <si>
+    <t>gonado, somato, thyreo, cortico, ADH</t>
+  </si>
+  <si>
+    <t>1.5ug/l</t>
+  </si>
+  <si>
+    <t>6.5nmol</t>
+  </si>
+  <si>
+    <t>Test 0.7</t>
+  </si>
+  <si>
+    <t>gonado, somato, thyreo, cortico</t>
+  </si>
+  <si>
+    <t>gonado, somato, thyreo</t>
+  </si>
+  <si>
+    <t>53.3ug/l</t>
+  </si>
+  <si>
+    <t>rest fehlt</t>
+  </si>
+  <si>
+    <t>750ug/l</t>
+  </si>
+  <si>
+    <t>88.2ug/l</t>
+  </si>
+  <si>
+    <t>22.1nmol</t>
+  </si>
+  <si>
+    <t>18.7ug/l</t>
+  </si>
+  <si>
+    <t>15.4nmol</t>
+  </si>
+  <si>
+    <t>11.3ug/l</t>
+  </si>
+  <si>
+    <t>22.3nmol</t>
+  </si>
+  <si>
+    <t>Testo 31.7nmol</t>
+  </si>
+  <si>
+    <t>5.2ug/l</t>
+  </si>
+  <si>
+    <t>43.1nmol</t>
+  </si>
+  <si>
+    <t>Testo 11.1nmol</t>
+  </si>
+  <si>
+    <t>100ug/l</t>
+  </si>
+  <si>
+    <t>extern Lareida, Prolaktin funktionell interpretiert</t>
+  </si>
+  <si>
+    <t>thyreo, gonado</t>
+  </si>
+  <si>
+    <t>thyreo, gonado, somato</t>
+  </si>
+  <si>
+    <t>null-zell</t>
+  </si>
+  <si>
+    <t>57ug/l</t>
+  </si>
+  <si>
+    <t>998ug/l</t>
+  </si>
+  <si>
+    <t>19.9nmol</t>
+  </si>
+  <si>
+    <t>Testo 3.9nmol</t>
+  </si>
+  <si>
+    <t>463ug/l</t>
+  </si>
+  <si>
+    <t>31.2nnol</t>
+  </si>
+  <si>
+    <t>10520mu/L</t>
+  </si>
+  <si>
+    <t>15nmol</t>
+  </si>
+  <si>
+    <t>19.6ug/l</t>
+  </si>
+  <si>
+    <t>16.2nmol/l</t>
+  </si>
+  <si>
+    <t>cortico, somato, gonado</t>
+  </si>
+  <si>
+    <t>0.6ug/l</t>
+  </si>
+  <si>
+    <t>extern Olten</t>
+  </si>
+  <si>
+    <t>11,2nmol</t>
+  </si>
+  <si>
+    <t>17,6nmol</t>
+  </si>
+  <si>
+    <t>Testo 8,3nmol/l</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>25.4nmol/l</t>
+  </si>
+  <si>
+    <t>FSH 123U/L, LH 35U/L</t>
+  </si>
+  <si>
+    <t>extern Zug, postmenopausal</t>
+  </si>
+  <si>
+    <t>kein Labor (extern wie intern)</t>
+  </si>
+  <si>
+    <t>extern (Lareida), kein präop Labor</t>
+  </si>
+  <si>
+    <t>gonado, cortico, thyreo, somato</t>
+  </si>
+  <si>
+    <t>gonado, cortico, thyreo</t>
+  </si>
+  <si>
+    <t>extern, kein Labor mehr (Endokrinologe in Pension)</t>
+  </si>
+  <si>
+    <t>Einblutung</t>
+  </si>
+  <si>
+    <t>Begrifferklärung</t>
+  </si>
+  <si>
+    <t>Gonado</t>
+  </si>
+  <si>
+    <t>Ausfall der gonadotropen Achse (LH, FSH), sprich Pat. hat zu wenige Geschlechtshormone</t>
+  </si>
+  <si>
+    <t>Ausfall der thyreotropen Achse (TSH), sprich Pat. hat zu wenige Schilddrüsenhormone</t>
+  </si>
+  <si>
+    <t>Ausfall der somatotropen Achse (GH), sprich Pat. hat zu wenige Wachstumshormone, sprich Leber produziert zuwenig IGF-1</t>
+  </si>
+  <si>
+    <t>Cortico</t>
+  </si>
+  <si>
+    <t>Ausfall der corticotropen Achse (ACTH), sprich Pat. hat zu wenige Cortisol/Stress-hormone</t>
+  </si>
+  <si>
+    <t>Ausfall der ADH Produktion im Hypophysen-Hinterlappen (sehr selten), sprich Pat. kann Urin nicht mehr genügend konzentrieren</t>
+  </si>
+  <si>
+    <t>Prä und Post</t>
+  </si>
+  <si>
+    <t>Mapping via Laborentnahmedatum und Operationsdatum möglich, prinzipiell würde ich diese Spalten mal ignorieren, mehr klinisch orientiert, um zu sehen, ob eine allfällige Operation bezgl. Hormonsituation erfolgreich war oder nicht</t>
+  </si>
+  <si>
+    <t>Labor-Einheiten</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/amamanualofstyle/si-conversion-calculator</t>
+  </si>
+  <si>
+    <t>Testosteron</t>
+  </si>
+  <si>
+    <t>100ng/dl</t>
+  </si>
+  <si>
+    <t>0.0347</t>
+  </si>
+  <si>
+    <t>3.47nmol/l</t>
+  </si>
+  <si>
+    <t>sollte immer in nmol/l sein in CH</t>
+  </si>
+  <si>
+    <t>128.71pmol/l</t>
+  </si>
+  <si>
+    <t>sollte immer in pmol/l sein in CH</t>
+  </si>
+  <si>
+    <t>IGF-1</t>
+  </si>
+  <si>
+    <t>100ng/ml</t>
+  </si>
+  <si>
+    <t>0.131</t>
+  </si>
+  <si>
+    <t>13.1nmol/l</t>
+  </si>
+  <si>
+    <t>Labor-Normwerte</t>
+  </si>
+  <si>
+    <t>Geschlechtshormone</t>
+  </si>
+  <si>
+    <t>vorerst ignorieren, da zu komplex (F: Zyklus, M: grosse individuelle Streuung)</t>
+  </si>
+  <si>
+    <t>siehe Tabelle 3</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5794073/</t>
+  </si>
+  <si>
+    <t>Tabelle 1, Median</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9206165/</t>
+  </si>
+  <si>
+    <t>im Stimulationstest (Cor30 oder Cor60) im Export sollte &gt;500nmol/l erreichen</t>
+  </si>
+  <si>
+    <t>Tabelle 2, Median</t>
+  </si>
+  <si>
+    <t>https://labosud.fr/wp-content/uploads/sites/7/2023/08/Verification_of_Roche_reference_ranges_for_serum_prolactin_in_children_adolescents_adults_and_the_elderly-2023-07-11-05-21.pdf</t>
+  </si>
+  <si>
+    <t>Beispiel-Patienten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prolaktinom PID </t>
+  </si>
+  <si>
+    <t>Non-Prolaktinom PID</t>
   </si>
 </sst>
 </file>
@@ -7540,7 +7946,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7569,8 +7975,25 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7586,6 +8009,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE95CFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -7625,10 +8054,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -7646,8 +8076,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -7989,14 +8425,18 @@
   <dimension ref="A1:W1199"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="E69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E69" sqref="E69"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="24" width="19.42578125" customWidth="1"/>
+    <col min="1" max="20" width="19.42578125" customWidth="1"/>
+    <col min="21" max="21" width="28" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="35" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -65499,8 +65939,8 @@
   <dimension ref="A1:AB527"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="I198" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P1" sqref="P1"/>
+      <pane ySplit="1" topLeftCell="I232" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M258" sqref="M258"/>
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -65891,7 +66331,7 @@
         <v>30</v>
       </c>
       <c r="L6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="S6" s="3">
         <v>44470</v>
@@ -66845,7 +67285,7 @@
         <v>32</v>
       </c>
       <c r="S22" s="3">
-        <v>45171</v>
+        <v>39845</v>
       </c>
       <c r="T22" s="3">
         <v>39862</v>
@@ -79198,10 +79638,10 @@
       <c r="J216" s="11">
         <v>300151985</v>
       </c>
-      <c r="K216" t="s">
+      <c r="L216" t="s">
         <v>2489</v>
       </c>
-      <c r="L216" t="s">
+      <c r="R216" t="s">
         <v>2490</v>
       </c>
       <c r="S216" s="3">
@@ -79335,7 +79775,7 @@
         <v>31</v>
       </c>
       <c r="V218" t="s">
-        <v>2493</v>
+        <v>33</v>
       </c>
       <c r="W218" t="s">
         <v>34</v>
@@ -79403,7 +79843,7 @@
         <v>40</v>
       </c>
       <c r="V219" t="s">
-        <v>2494</v>
+        <v>2493</v>
       </c>
       <c r="W219" t="s">
         <v>34</v>
@@ -79509,7 +79949,7 @@
         <v>30</v>
       </c>
       <c r="L221" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
       <c r="S221" s="3">
         <v>42767</v>
@@ -79521,7 +79961,7 @@
         <v>2442</v>
       </c>
       <c r="V221" t="s">
-        <v>2496</v>
+        <v>2495</v>
       </c>
       <c r="W221" t="s">
         <v>34</v>
@@ -79577,10 +80017,10 @@
         <v>30</v>
       </c>
       <c r="L222" t="s">
-        <v>2497</v>
-      </c>
-      <c r="U222" t="s">
-        <v>40</v>
+        <v>2496</v>
+      </c>
+      <c r="S222" s="3">
+        <v>43922</v>
       </c>
       <c r="V222" t="s">
         <v>157</v>
@@ -79632,8 +80072,11 @@
       <c r="I223" t="s">
         <v>29</v>
       </c>
-      <c r="J223" s="12">
+      <c r="J223">
         <v>300043953</v>
+      </c>
+      <c r="R223" t="s">
+        <v>2484</v>
       </c>
       <c r="X223">
         <v>18</v>
@@ -79679,8 +80122,29 @@
       <c r="I224" t="s">
         <v>29</v>
       </c>
-      <c r="J224" s="12">
+      <c r="J224">
         <v>300116322</v>
+      </c>
+      <c r="K224" t="s">
+        <v>30</v>
+      </c>
+      <c r="L224" t="s">
+        <v>2497</v>
+      </c>
+      <c r="S224" s="3">
+        <v>41638</v>
+      </c>
+      <c r="T224" s="3">
+        <v>43339</v>
+      </c>
+      <c r="U224" t="s">
+        <v>2498</v>
+      </c>
+      <c r="V224" t="s">
+        <v>60</v>
+      </c>
+      <c r="W224" t="s">
+        <v>157</v>
       </c>
       <c r="X224">
         <v>64</v>
@@ -79726,8 +80190,29 @@
       <c r="I225" t="s">
         <v>29</v>
       </c>
-      <c r="J225" s="12">
+      <c r="J225">
         <v>743011</v>
+      </c>
+      <c r="K225" t="s">
+        <v>2499</v>
+      </c>
+      <c r="L225" t="s">
+        <v>2500</v>
+      </c>
+      <c r="S225" s="3">
+        <v>41924</v>
+      </c>
+      <c r="T225" s="3">
+        <v>41925</v>
+      </c>
+      <c r="U225" t="s">
+        <v>40</v>
+      </c>
+      <c r="V225" t="s">
+        <v>2501</v>
+      </c>
+      <c r="W225" t="s">
+        <v>34</v>
       </c>
       <c r="X225">
         <v>62</v>
@@ -79773,8 +80258,11 @@
       <c r="I226" t="s">
         <v>29</v>
       </c>
-      <c r="J226" s="12">
+      <c r="J226">
         <v>300191364</v>
+      </c>
+      <c r="R226" t="s">
+        <v>2502</v>
       </c>
       <c r="X226">
         <v>28</v>
@@ -79820,8 +80308,29 @@
       <c r="I227" t="s">
         <v>29</v>
       </c>
-      <c r="J227" s="12">
+      <c r="J227">
         <v>430419</v>
+      </c>
+      <c r="K227" t="s">
+        <v>30</v>
+      </c>
+      <c r="L227" t="s">
+        <v>2503</v>
+      </c>
+      <c r="S227" s="3">
+        <v>41393</v>
+      </c>
+      <c r="T227" s="3">
+        <v>41509</v>
+      </c>
+      <c r="U227" t="s">
+        <v>40</v>
+      </c>
+      <c r="V227" t="s">
+        <v>60</v>
+      </c>
+      <c r="W227" t="s">
+        <v>34</v>
       </c>
       <c r="X227">
         <v>67</v>
@@ -79867,8 +80376,11 @@
       <c r="I228" t="s">
         <v>29</v>
       </c>
-      <c r="J228" s="12">
+      <c r="J228">
         <v>300090571</v>
+      </c>
+      <c r="R228" t="s">
+        <v>2504</v>
       </c>
       <c r="X228">
         <v>25</v>
@@ -79914,8 +80426,23 @@
       <c r="I229" t="s">
         <v>29</v>
       </c>
-      <c r="J229" s="12">
+      <c r="J229">
         <v>743647</v>
+      </c>
+      <c r="L229" t="s">
+        <v>60</v>
+      </c>
+      <c r="R229" t="s">
+        <v>2505</v>
+      </c>
+      <c r="S229" s="3">
+        <v>43941</v>
+      </c>
+      <c r="V229" t="s">
+        <v>96</v>
+      </c>
+      <c r="W229" t="s">
+        <v>34</v>
       </c>
       <c r="X229">
         <v>49</v>
@@ -79961,8 +80488,11 @@
       <c r="I230" t="s">
         <v>29</v>
       </c>
-      <c r="J230" s="12">
+      <c r="J230">
         <v>733215</v>
+      </c>
+      <c r="R230" s="17" t="s">
+        <v>2506</v>
       </c>
       <c r="X230">
         <v>6</v>
@@ -80008,8 +80538,23 @@
       <c r="I231" t="s">
         <v>29</v>
       </c>
-      <c r="J231" s="12">
+      <c r="J231">
         <v>74960</v>
+      </c>
+      <c r="K231" t="s">
+        <v>30</v>
+      </c>
+      <c r="L231" t="s">
+        <v>32</v>
+      </c>
+      <c r="S231" s="3">
+        <v>43951</v>
+      </c>
+      <c r="V231" t="s">
+        <v>2507</v>
+      </c>
+      <c r="W231" t="s">
+        <v>157</v>
       </c>
       <c r="X231">
         <v>72</v>
@@ -80055,8 +80600,29 @@
       <c r="I232" t="s">
         <v>29</v>
       </c>
-      <c r="J232" s="12">
+      <c r="J232">
         <v>443533</v>
+      </c>
+      <c r="K232" t="s">
+        <v>30</v>
+      </c>
+      <c r="L232" t="s">
+        <v>2508</v>
+      </c>
+      <c r="S232" s="3">
+        <v>42591</v>
+      </c>
+      <c r="T232" s="3">
+        <v>42601</v>
+      </c>
+      <c r="U232" t="s">
+        <v>40</v>
+      </c>
+      <c r="V232" t="s">
+        <v>60</v>
+      </c>
+      <c r="W232" t="s">
+        <v>34</v>
       </c>
       <c r="X232">
         <v>84</v>
@@ -80102,8 +80668,17 @@
       <c r="I233" t="s">
         <v>29</v>
       </c>
-      <c r="J233" s="12">
+      <c r="J233">
         <v>300189422</v>
+      </c>
+      <c r="K233" t="s">
+        <v>53</v>
+      </c>
+      <c r="R233" t="s">
+        <v>2509</v>
+      </c>
+      <c r="S233" s="3">
+        <v>44296</v>
       </c>
       <c r="X233">
         <v>26</v>
@@ -80149,8 +80724,29 @@
       <c r="I234" t="s">
         <v>29</v>
       </c>
-      <c r="J234" s="12">
+      <c r="J234">
         <v>615553</v>
+      </c>
+      <c r="K234" t="s">
+        <v>30</v>
+      </c>
+      <c r="L234" t="s">
+        <v>2510</v>
+      </c>
+      <c r="S234" s="3">
+        <v>40631</v>
+      </c>
+      <c r="T234" s="3">
+        <v>40632</v>
+      </c>
+      <c r="U234" t="s">
+        <v>2442</v>
+      </c>
+      <c r="V234" t="s">
+        <v>60</v>
+      </c>
+      <c r="W234" t="s">
+        <v>34</v>
       </c>
       <c r="X234">
         <v>67</v>
@@ -80196,8 +80792,20 @@
       <c r="I235" t="s">
         <v>29</v>
       </c>
-      <c r="J235" s="12">
+      <c r="J235">
         <v>220057</v>
+      </c>
+      <c r="R235" t="s">
+        <v>2505</v>
+      </c>
+      <c r="S235" s="3">
+        <v>44292</v>
+      </c>
+      <c r="V235" t="s">
+        <v>96</v>
+      </c>
+      <c r="W235" t="s">
+        <v>34</v>
       </c>
       <c r="X235">
         <v>44</v>
@@ -80243,8 +80851,26 @@
       <c r="I236" t="s">
         <v>29</v>
       </c>
-      <c r="J236" s="12">
+      <c r="J236">
         <v>770245</v>
+      </c>
+      <c r="L236" t="s">
+        <v>60</v>
+      </c>
+      <c r="R236" t="s">
+        <v>2505</v>
+      </c>
+      <c r="S236" s="3">
+        <v>43361</v>
+      </c>
+      <c r="T236" s="3">
+        <v>44237</v>
+      </c>
+      <c r="V236" t="s">
+        <v>96</v>
+      </c>
+      <c r="W236" t="s">
+        <v>34</v>
       </c>
       <c r="X236">
         <v>40</v>
@@ -80290,8 +80916,23 @@
       <c r="I237" t="s">
         <v>29</v>
       </c>
-      <c r="J237" s="12">
+      <c r="J237">
         <v>7375</v>
+      </c>
+      <c r="K237" t="s">
+        <v>53</v>
+      </c>
+      <c r="L237" t="s">
+        <v>2511</v>
+      </c>
+      <c r="S237" s="3">
+        <v>44282</v>
+      </c>
+      <c r="V237" t="s">
+        <v>60</v>
+      </c>
+      <c r="W237" t="s">
+        <v>34</v>
       </c>
       <c r="X237">
         <v>55</v>
@@ -80337,8 +80978,23 @@
       <c r="I238" t="s">
         <v>29</v>
       </c>
-      <c r="J238" s="12">
+      <c r="J238">
         <v>613086</v>
+      </c>
+      <c r="K238" t="s">
+        <v>53</v>
+      </c>
+      <c r="L238" t="s">
+        <v>60</v>
+      </c>
+      <c r="S238" s="3">
+        <v>40544</v>
+      </c>
+      <c r="V238" t="s">
+        <v>60</v>
+      </c>
+      <c r="W238" t="s">
+        <v>34</v>
       </c>
       <c r="X238">
         <v>34</v>
@@ -80384,8 +81040,23 @@
       <c r="I239" t="s">
         <v>29</v>
       </c>
-      <c r="J239" s="12">
+      <c r="J239">
         <v>300018685</v>
+      </c>
+      <c r="K239" t="s">
+        <v>53</v>
+      </c>
+      <c r="L239" t="s">
+        <v>60</v>
+      </c>
+      <c r="S239" s="3">
+        <v>42478</v>
+      </c>
+      <c r="V239" t="s">
+        <v>60</v>
+      </c>
+      <c r="W239" t="s">
+        <v>34</v>
       </c>
       <c r="X239">
         <v>38</v>
@@ -80431,8 +81102,23 @@
       <c r="I240" t="s">
         <v>29</v>
       </c>
-      <c r="J240" s="12">
+      <c r="J240">
         <v>20164</v>
+      </c>
+      <c r="L240" t="s">
+        <v>60</v>
+      </c>
+      <c r="R240" t="s">
+        <v>2505</v>
+      </c>
+      <c r="S240" s="3">
+        <v>43237</v>
+      </c>
+      <c r="V240" t="s">
+        <v>2512</v>
+      </c>
+      <c r="W240" t="s">
+        <v>34</v>
       </c>
       <c r="X240">
         <v>35</v>
@@ -80478,8 +81164,23 @@
       <c r="I241" t="s">
         <v>29</v>
       </c>
-      <c r="J241" s="12">
+      <c r="J241">
         <v>300101347</v>
+      </c>
+      <c r="K241" t="s">
+        <v>53</v>
+      </c>
+      <c r="L241" t="s">
+        <v>60</v>
+      </c>
+      <c r="S241" s="3">
+        <v>43277</v>
+      </c>
+      <c r="V241" t="s">
+        <v>60</v>
+      </c>
+      <c r="W241" t="s">
+        <v>34</v>
       </c>
       <c r="X241">
         <v>40</v>
@@ -80525,8 +81226,23 @@
       <c r="I242" t="s">
         <v>29</v>
       </c>
-      <c r="J242" s="12">
+      <c r="J242">
         <v>636550</v>
+      </c>
+      <c r="K242" t="s">
+        <v>30</v>
+      </c>
+      <c r="L242" t="s">
+        <v>2513</v>
+      </c>
+      <c r="S242" s="3">
+        <v>40848</v>
+      </c>
+      <c r="V242" t="s">
+        <v>60</v>
+      </c>
+      <c r="W242" t="s">
+        <v>157</v>
       </c>
       <c r="X242">
         <v>50</v>
@@ -80572,8 +81288,26 @@
       <c r="I243" t="s">
         <v>29</v>
       </c>
-      <c r="J243" s="12">
+      <c r="J243">
         <v>20374</v>
+      </c>
+      <c r="K243" t="s">
+        <v>53</v>
+      </c>
+      <c r="L243" t="s">
+        <v>60</v>
+      </c>
+      <c r="R243" t="s">
+        <v>2514</v>
+      </c>
+      <c r="S243" s="3">
+        <v>43864</v>
+      </c>
+      <c r="V243" t="s">
+        <v>60</v>
+      </c>
+      <c r="W243" t="s">
+        <v>34</v>
       </c>
       <c r="X243">
         <v>32</v>
@@ -80619,8 +81353,11 @@
       <c r="I244" t="s">
         <v>29</v>
       </c>
-      <c r="J244" s="12">
+      <c r="J244">
         <v>590059</v>
+      </c>
+      <c r="R244" t="s">
+        <v>2484</v>
       </c>
       <c r="X244">
         <v>30</v>
@@ -80666,8 +81403,11 @@
       <c r="I245" t="s">
         <v>29</v>
       </c>
-      <c r="J245" s="12">
+      <c r="J245">
         <v>300176139</v>
+      </c>
+      <c r="R245" t="s">
+        <v>2515</v>
       </c>
       <c r="X245">
         <v>29</v>
@@ -80713,8 +81453,14 @@
       <c r="I246" t="s">
         <v>29</v>
       </c>
-      <c r="J246" s="12">
+      <c r="J246">
         <v>300184337</v>
+      </c>
+      <c r="R246" t="s">
+        <v>2484</v>
+      </c>
+      <c r="S246" s="3">
+        <v>44250</v>
       </c>
       <c r="X246">
         <v>45</v>
@@ -80760,8 +81506,23 @@
       <c r="I247" t="s">
         <v>196</v>
       </c>
-      <c r="J247" s="12">
+      <c r="J247">
         <v>300241712</v>
+      </c>
+      <c r="K247" t="s">
+        <v>30</v>
+      </c>
+      <c r="L247" t="s">
+        <v>2516</v>
+      </c>
+      <c r="S247" s="3">
+        <v>44246</v>
+      </c>
+      <c r="V247" t="s">
+        <v>2517</v>
+      </c>
+      <c r="W247" t="s">
+        <v>157</v>
       </c>
       <c r="X247">
         <v>72</v>
@@ -80807,8 +81568,14 @@
       <c r="I248" t="s">
         <v>29</v>
       </c>
-      <c r="J248" s="12">
+      <c r="J248" s="11">
         <v>631002</v>
+      </c>
+      <c r="K248" t="s">
+        <v>53</v>
+      </c>
+      <c r="S248" s="3">
+        <v>44239</v>
       </c>
       <c r="X248">
         <v>34</v>
@@ -80854,8 +81621,23 @@
       <c r="I249" t="s">
         <v>29</v>
       </c>
-      <c r="J249" s="12">
+      <c r="J249">
         <v>717330</v>
+      </c>
+      <c r="K249" t="s">
+        <v>30</v>
+      </c>
+      <c r="L249" t="s">
+        <v>2518</v>
+      </c>
+      <c r="S249" s="3">
+        <v>41689</v>
+      </c>
+      <c r="V249" t="s">
+        <v>2517</v>
+      </c>
+      <c r="W249" t="s">
+        <v>157</v>
       </c>
       <c r="X249">
         <v>55</v>
@@ -88142,6 +88924,36 @@
       <c r="J404" s="12">
         <v>560863</v>
       </c>
+      <c r="K404" t="s">
+        <v>53</v>
+      </c>
+      <c r="L404" t="s">
+        <v>32</v>
+      </c>
+      <c r="M404" t="s">
+        <v>2519</v>
+      </c>
+      <c r="N404" t="s">
+        <v>2520</v>
+      </c>
+      <c r="O404">
+        <v>607</v>
+      </c>
+      <c r="P404">
+        <v>11.4</v>
+      </c>
+      <c r="S404" s="3">
+        <v>42795</v>
+      </c>
+      <c r="U404" t="s">
+        <v>40</v>
+      </c>
+      <c r="V404" t="s">
+        <v>157</v>
+      </c>
+      <c r="W404" t="s">
+        <v>157</v>
+      </c>
       <c r="X404">
         <v>23</v>
       </c>
@@ -88189,6 +89001,39 @@
       <c r="J405" s="12">
         <v>459429</v>
       </c>
+      <c r="K405" t="s">
+        <v>30</v>
+      </c>
+      <c r="L405" t="s">
+        <v>40</v>
+      </c>
+      <c r="M405" t="s">
+        <v>2521</v>
+      </c>
+      <c r="N405" t="s">
+        <v>2522</v>
+      </c>
+      <c r="O405">
+        <v>703</v>
+      </c>
+      <c r="P405">
+        <v>13.2</v>
+      </c>
+      <c r="S405" s="3">
+        <v>42887</v>
+      </c>
+      <c r="T405" s="3">
+        <v>42984</v>
+      </c>
+      <c r="U405" t="s">
+        <v>40</v>
+      </c>
+      <c r="V405" t="s">
+        <v>42</v>
+      </c>
+      <c r="W405" t="s">
+        <v>34</v>
+      </c>
       <c r="X405">
         <v>52</v>
       </c>
@@ -88236,6 +89081,9 @@
       <c r="J406" s="12">
         <v>300127746</v>
       </c>
+      <c r="R406" t="s">
+        <v>2484</v>
+      </c>
       <c r="X406">
         <v>68</v>
       </c>
@@ -88283,6 +89131,9 @@
       <c r="J407" s="12">
         <v>300022448</v>
       </c>
+      <c r="R407" t="s">
+        <v>2484</v>
+      </c>
       <c r="X407">
         <v>75</v>
       </c>
@@ -88330,6 +89181,33 @@
       <c r="J408" s="12">
         <v>580485</v>
       </c>
+      <c r="K408" t="s">
+        <v>30</v>
+      </c>
+      <c r="L408" t="s">
+        <v>40</v>
+      </c>
+      <c r="M408" t="s">
+        <v>2523</v>
+      </c>
+      <c r="O408">
+        <v>524</v>
+      </c>
+      <c r="S408" s="3">
+        <v>40269</v>
+      </c>
+      <c r="T408" s="3">
+        <v>40299</v>
+      </c>
+      <c r="U408" t="s">
+        <v>40</v>
+      </c>
+      <c r="V408" t="s">
+        <v>60</v>
+      </c>
+      <c r="W408" t="s">
+        <v>34</v>
+      </c>
       <c r="X408">
         <v>62</v>
       </c>
@@ -88377,6 +89255,9 @@
       <c r="J409" s="12">
         <v>356919</v>
       </c>
+      <c r="R409" t="s">
+        <v>2484</v>
+      </c>
       <c r="X409">
         <v>69</v>
       </c>
@@ -88424,6 +89305,36 @@
       <c r="J410" s="12">
         <v>17081</v>
       </c>
+      <c r="K410" t="s">
+        <v>53</v>
+      </c>
+      <c r="L410" t="s">
+        <v>40</v>
+      </c>
+      <c r="M410" t="s">
+        <v>2524</v>
+      </c>
+      <c r="N410" t="s">
+        <v>2525</v>
+      </c>
+      <c r="O410">
+        <v>766</v>
+      </c>
+      <c r="P410">
+        <v>14.3</v>
+      </c>
+      <c r="S410" s="3">
+        <v>42309</v>
+      </c>
+      <c r="U410" t="s">
+        <v>40</v>
+      </c>
+      <c r="V410" t="s">
+        <v>60</v>
+      </c>
+      <c r="W410" t="s">
+        <v>34</v>
+      </c>
       <c r="X410">
         <v>59</v>
       </c>
@@ -88471,6 +89382,9 @@
       <c r="J411" s="12">
         <v>63087</v>
       </c>
+      <c r="R411" t="s">
+        <v>2484</v>
+      </c>
       <c r="X411">
         <v>58</v>
       </c>
@@ -88518,6 +89432,30 @@
       <c r="J412" s="12">
         <v>300081806</v>
       </c>
+      <c r="K412" t="s">
+        <v>30</v>
+      </c>
+      <c r="L412" s="7" t="s">
+        <v>2526</v>
+      </c>
+      <c r="R412" t="s">
+        <v>2527</v>
+      </c>
+      <c r="S412" s="3">
+        <v>43014</v>
+      </c>
+      <c r="T412" s="3">
+        <v>43025</v>
+      </c>
+      <c r="U412" t="s">
+        <v>2526</v>
+      </c>
+      <c r="V412" t="s">
+        <v>60</v>
+      </c>
+      <c r="W412" t="s">
+        <v>34</v>
+      </c>
       <c r="X412">
         <v>71</v>
       </c>
@@ -88565,6 +89503,30 @@
       <c r="J413" s="12">
         <v>591096</v>
       </c>
+      <c r="K413" t="s">
+        <v>30</v>
+      </c>
+      <c r="L413" t="s">
+        <v>182</v>
+      </c>
+      <c r="M413" t="s">
+        <v>2528</v>
+      </c>
+      <c r="S413" s="3">
+        <v>40330</v>
+      </c>
+      <c r="T413" s="3">
+        <v>40339</v>
+      </c>
+      <c r="U413" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="V413" t="s">
+        <v>33</v>
+      </c>
+      <c r="W413" t="s">
+        <v>34</v>
+      </c>
       <c r="X413">
         <v>56</v>
       </c>
@@ -88612,6 +89574,15 @@
       <c r="J414" s="12">
         <v>300120796</v>
       </c>
+      <c r="K414" t="s">
+        <v>2465</v>
+      </c>
+      <c r="V414" t="s">
+        <v>2529</v>
+      </c>
+      <c r="W414" t="s">
+        <v>2529</v>
+      </c>
       <c r="X414">
         <v>19</v>
       </c>
@@ -88659,6 +89630,15 @@
       <c r="J415" s="12">
         <v>300057765</v>
       </c>
+      <c r="K415" t="s">
+        <v>2465</v>
+      </c>
+      <c r="V415" t="s">
+        <v>2529</v>
+      </c>
+      <c r="W415" t="s">
+        <v>2529</v>
+      </c>
       <c r="X415">
         <v>62</v>
       </c>
@@ -88706,6 +89686,15 @@
       <c r="J416" s="12">
         <v>516450</v>
       </c>
+      <c r="K416" t="s">
+        <v>2465</v>
+      </c>
+      <c r="V416" t="s">
+        <v>2529</v>
+      </c>
+      <c r="W416" t="s">
+        <v>2529</v>
+      </c>
       <c r="X416">
         <v>34</v>
       </c>
@@ -88753,6 +89742,9 @@
       <c r="J417" s="12">
         <v>239507</v>
       </c>
+      <c r="R417" t="s">
+        <v>2484</v>
+      </c>
       <c r="X417">
         <v>61</v>
       </c>
@@ -88800,6 +89792,30 @@
       <c r="J418" s="12">
         <v>277197</v>
       </c>
+      <c r="K418" t="s">
+        <v>53</v>
+      </c>
+      <c r="L418" t="s">
+        <v>117</v>
+      </c>
+      <c r="M418" t="s">
+        <v>2530</v>
+      </c>
+      <c r="S418" s="3">
+        <v>38777</v>
+      </c>
+      <c r="T418" s="3">
+        <v>39898</v>
+      </c>
+      <c r="U418" t="s">
+        <v>40</v>
+      </c>
+      <c r="V418" t="s">
+        <v>157</v>
+      </c>
+      <c r="W418" t="s">
+        <v>157</v>
+      </c>
       <c r="X418">
         <v>47</v>
       </c>
@@ -88847,6 +89863,33 @@
       <c r="J419" s="12">
         <v>300063047</v>
       </c>
+      <c r="K419" t="s">
+        <v>53</v>
+      </c>
+      <c r="L419" t="s">
+        <v>40</v>
+      </c>
+      <c r="N419" t="s">
+        <v>2531</v>
+      </c>
+      <c r="O419">
+        <v>532</v>
+      </c>
+      <c r="P419">
+        <v>18</v>
+      </c>
+      <c r="S419" s="3">
+        <v>42745</v>
+      </c>
+      <c r="T419" s="3">
+        <v>42963</v>
+      </c>
+      <c r="V419" t="s">
+        <v>42</v>
+      </c>
+      <c r="W419" t="s">
+        <v>34</v>
+      </c>
       <c r="X419">
         <v>72</v>
       </c>
@@ -88894,6 +89937,27 @@
       <c r="J420" s="12">
         <v>416558</v>
       </c>
+      <c r="K420" t="s">
+        <v>53</v>
+      </c>
+      <c r="L420" t="s">
+        <v>32</v>
+      </c>
+      <c r="R420" t="s">
+        <v>2527</v>
+      </c>
+      <c r="S420" s="3">
+        <v>42418</v>
+      </c>
+      <c r="U420" t="s">
+        <v>32</v>
+      </c>
+      <c r="V420" t="s">
+        <v>96</v>
+      </c>
+      <c r="W420" t="s">
+        <v>34</v>
+      </c>
       <c r="X420">
         <v>51</v>
       </c>
@@ -88941,6 +90005,15 @@
       <c r="J421" s="12">
         <v>652892</v>
       </c>
+      <c r="K421" t="s">
+        <v>2465</v>
+      </c>
+      <c r="V421" t="s">
+        <v>2529</v>
+      </c>
+      <c r="W421" t="s">
+        <v>2529</v>
+      </c>
       <c r="X421">
         <v>68</v>
       </c>
@@ -88988,6 +90061,9 @@
       <c r="J422" s="12">
         <v>298076</v>
       </c>
+      <c r="R422" t="s">
+        <v>2484</v>
+      </c>
       <c r="X422">
         <v>70</v>
       </c>
@@ -89035,6 +90111,24 @@
       <c r="J423" s="12">
         <v>579143</v>
       </c>
+      <c r="K423" t="s">
+        <v>30</v>
+      </c>
+      <c r="L423" t="s">
+        <v>103</v>
+      </c>
+      <c r="S423" s="3">
+        <v>33604</v>
+      </c>
+      <c r="U423" t="s">
+        <v>32</v>
+      </c>
+      <c r="V423" t="s">
+        <v>157</v>
+      </c>
+      <c r="W423" t="s">
+        <v>157</v>
+      </c>
       <c r="X423">
         <v>48</v>
       </c>
@@ -89082,6 +90176,9 @@
       <c r="J424" s="12">
         <v>234316</v>
       </c>
+      <c r="R424" t="s">
+        <v>2484</v>
+      </c>
       <c r="X424">
         <v>48</v>
       </c>
@@ -89129,6 +90226,15 @@
       <c r="J425" s="12">
         <v>206301</v>
       </c>
+      <c r="K425" t="s">
+        <v>2465</v>
+      </c>
+      <c r="V425" t="s">
+        <v>2529</v>
+      </c>
+      <c r="W425" t="s">
+        <v>2529</v>
+      </c>
       <c r="X425">
         <v>27</v>
       </c>
@@ -89176,6 +90282,36 @@
       <c r="J426" s="12">
         <v>112374</v>
       </c>
+      <c r="K426" t="s">
+        <v>30</v>
+      </c>
+      <c r="L426" t="s">
+        <v>32</v>
+      </c>
+      <c r="M426" t="s">
+        <v>2532</v>
+      </c>
+      <c r="N426" t="s">
+        <v>2533</v>
+      </c>
+      <c r="O426">
+        <v>334</v>
+      </c>
+      <c r="P426">
+        <v>11</v>
+      </c>
+      <c r="Q426" t="s">
+        <v>2534</v>
+      </c>
+      <c r="S426" s="3">
+        <v>40575</v>
+      </c>
+      <c r="V426" t="s">
+        <v>157</v>
+      </c>
+      <c r="W426" t="s">
+        <v>157</v>
+      </c>
       <c r="X426">
         <v>78</v>
       </c>
@@ -89223,6 +90359,39 @@
       <c r="J427" s="12">
         <v>113792</v>
       </c>
+      <c r="K427" t="s">
+        <v>30</v>
+      </c>
+      <c r="L427" t="s">
+        <v>32</v>
+      </c>
+      <c r="M427" t="s">
+        <v>2535</v>
+      </c>
+      <c r="N427" t="s">
+        <v>2536</v>
+      </c>
+      <c r="O427">
+        <v>1380</v>
+      </c>
+      <c r="P427">
+        <v>11.8</v>
+      </c>
+      <c r="Q427" t="s">
+        <v>2537</v>
+      </c>
+      <c r="S427" s="3">
+        <v>41395</v>
+      </c>
+      <c r="U427" t="s">
+        <v>40</v>
+      </c>
+      <c r="V427" t="s">
+        <v>157</v>
+      </c>
+      <c r="W427" t="s">
+        <v>157</v>
+      </c>
       <c r="X427">
         <v>48</v>
       </c>
@@ -89270,6 +90439,33 @@
       <c r="J428" s="12">
         <v>542706</v>
       </c>
+      <c r="K428" t="s">
+        <v>30</v>
+      </c>
+      <c r="L428" t="s">
+        <v>130</v>
+      </c>
+      <c r="M428" t="s">
+        <v>2538</v>
+      </c>
+      <c r="O428">
+        <v>630</v>
+      </c>
+      <c r="R428" t="s">
+        <v>2539</v>
+      </c>
+      <c r="T428" s="3">
+        <v>39797</v>
+      </c>
+      <c r="U428" t="s">
+        <v>130</v>
+      </c>
+      <c r="V428" t="s">
+        <v>33</v>
+      </c>
+      <c r="W428" t="s">
+        <v>34</v>
+      </c>
       <c r="X428">
         <v>71</v>
       </c>
@@ -89317,6 +90513,9 @@
       <c r="J429" s="12">
         <v>629487</v>
       </c>
+      <c r="R429" t="s">
+        <v>2484</v>
+      </c>
       <c r="X429">
         <v>56</v>
       </c>
@@ -89364,6 +90563,9 @@
       <c r="J430" s="12">
         <v>263752</v>
       </c>
+      <c r="R430" t="s">
+        <v>2484</v>
+      </c>
       <c r="X430">
         <v>53</v>
       </c>
@@ -89411,6 +90613,39 @@
       <c r="J431" s="12">
         <v>242880</v>
       </c>
+      <c r="K431" t="s">
+        <v>30</v>
+      </c>
+      <c r="L431" t="s">
+        <v>32</v>
+      </c>
+      <c r="M431" t="s">
+        <v>2540</v>
+      </c>
+      <c r="N431" t="s">
+        <v>2541</v>
+      </c>
+      <c r="O431">
+        <v>1213</v>
+      </c>
+      <c r="P431">
+        <v>17</v>
+      </c>
+      <c r="Q431" t="s">
+        <v>2542</v>
+      </c>
+      <c r="S431" s="3">
+        <v>43090</v>
+      </c>
+      <c r="U431" t="s">
+        <v>40</v>
+      </c>
+      <c r="V431" t="s">
+        <v>157</v>
+      </c>
+      <c r="W431" t="s">
+        <v>157</v>
+      </c>
       <c r="X431">
         <v>83</v>
       </c>
@@ -89458,6 +90693,15 @@
       <c r="J432" s="12">
         <v>732030</v>
       </c>
+      <c r="K432" t="s">
+        <v>2465</v>
+      </c>
+      <c r="V432" t="s">
+        <v>2529</v>
+      </c>
+      <c r="W432" t="s">
+        <v>2529</v>
+      </c>
       <c r="X432">
         <v>35</v>
       </c>
@@ -89505,6 +90749,9 @@
       <c r="J433" s="12">
         <v>90307</v>
       </c>
+      <c r="R433" t="s">
+        <v>2484</v>
+      </c>
       <c r="X433">
         <v>52</v>
       </c>
@@ -89552,6 +90799,36 @@
       <c r="J434" s="12">
         <v>431742</v>
       </c>
+      <c r="K434" t="s">
+        <v>30</v>
+      </c>
+      <c r="L434" t="s">
+        <v>2543</v>
+      </c>
+      <c r="M434" t="s">
+        <v>2544</v>
+      </c>
+      <c r="O434">
+        <v>221</v>
+      </c>
+      <c r="Q434" t="s">
+        <v>2545</v>
+      </c>
+      <c r="S434" s="3">
+        <v>38412</v>
+      </c>
+      <c r="T434" s="3">
+        <v>38428</v>
+      </c>
+      <c r="U434" t="s">
+        <v>2546</v>
+      </c>
+      <c r="V434" t="s">
+        <v>33</v>
+      </c>
+      <c r="W434" t="s">
+        <v>34</v>
+      </c>
       <c r="X434">
         <v>77</v>
       </c>
@@ -89599,6 +90876,39 @@
       <c r="J435" s="12">
         <v>159059</v>
       </c>
+      <c r="K435" t="s">
+        <v>30</v>
+      </c>
+      <c r="L435" t="s">
+        <v>2547</v>
+      </c>
+      <c r="M435" t="s">
+        <v>2548</v>
+      </c>
+      <c r="N435" t="s">
+        <v>2549</v>
+      </c>
+      <c r="O435">
+        <v>280</v>
+      </c>
+      <c r="P435">
+        <v>6.7</v>
+      </c>
+      <c r="Q435" t="s">
+        <v>2550</v>
+      </c>
+      <c r="S435" s="3">
+        <v>40941</v>
+      </c>
+      <c r="U435" t="s">
+        <v>2551</v>
+      </c>
+      <c r="V435" t="s">
+        <v>60</v>
+      </c>
+      <c r="W435" t="s">
+        <v>34</v>
+      </c>
       <c r="X435">
         <v>79</v>
       </c>
@@ -89646,6 +90956,27 @@
       <c r="J436" s="12">
         <v>100762</v>
       </c>
+      <c r="K436" t="s">
+        <v>30</v>
+      </c>
+      <c r="L436" t="s">
+        <v>2552</v>
+      </c>
+      <c r="S436" s="3">
+        <v>34516</v>
+      </c>
+      <c r="T436" s="3">
+        <v>34547</v>
+      </c>
+      <c r="U436" t="s">
+        <v>2552</v>
+      </c>
+      <c r="V436" t="s">
+        <v>157</v>
+      </c>
+      <c r="W436" t="s">
+        <v>157</v>
+      </c>
       <c r="X436">
         <v>66</v>
       </c>
@@ -89693,6 +91024,15 @@
       <c r="J437" s="12">
         <v>82037</v>
       </c>
+      <c r="K437" t="s">
+        <v>2465</v>
+      </c>
+      <c r="V437" t="s">
+        <v>2529</v>
+      </c>
+      <c r="W437" t="s">
+        <v>2529</v>
+      </c>
       <c r="X437">
         <v>80</v>
       </c>
@@ -89740,6 +91080,33 @@
       <c r="J438" s="12">
         <v>137989</v>
       </c>
+      <c r="K438" t="s">
+        <v>53</v>
+      </c>
+      <c r="L438" t="s">
+        <v>32</v>
+      </c>
+      <c r="M438" t="s">
+        <v>2553</v>
+      </c>
+      <c r="O438">
+        <v>452</v>
+      </c>
+      <c r="Q438" t="s">
+        <v>2554</v>
+      </c>
+      <c r="S438" s="3">
+        <v>39234</v>
+      </c>
+      <c r="T438" s="3">
+        <v>39258</v>
+      </c>
+      <c r="V438" t="s">
+        <v>157</v>
+      </c>
+      <c r="W438" t="s">
+        <v>157</v>
+      </c>
       <c r="X438">
         <v>32</v>
       </c>
@@ -89787,6 +91154,33 @@
       <c r="J439" s="12">
         <v>62907</v>
       </c>
+      <c r="K439" t="s">
+        <v>30</v>
+      </c>
+      <c r="L439" t="s">
+        <v>32</v>
+      </c>
+      <c r="M439" t="s">
+        <v>2555</v>
+      </c>
+      <c r="O439">
+        <v>535</v>
+      </c>
+      <c r="Q439" t="s">
+        <v>2554</v>
+      </c>
+      <c r="S439" s="3">
+        <v>39853</v>
+      </c>
+      <c r="T439" s="3">
+        <v>39871</v>
+      </c>
+      <c r="V439" t="s">
+        <v>157</v>
+      </c>
+      <c r="W439" t="s">
+        <v>157</v>
+      </c>
       <c r="X439">
         <v>72</v>
       </c>
@@ -89834,6 +91228,27 @@
       <c r="J440" s="12">
         <v>431894</v>
       </c>
+      <c r="K440" t="s">
+        <v>30</v>
+      </c>
+      <c r="L440" t="s">
+        <v>32</v>
+      </c>
+      <c r="S440" s="3">
+        <v>43165</v>
+      </c>
+      <c r="T440" s="3">
+        <v>43168</v>
+      </c>
+      <c r="U440" t="s">
+        <v>32</v>
+      </c>
+      <c r="V440" t="s">
+        <v>157</v>
+      </c>
+      <c r="W440" t="s">
+        <v>157</v>
+      </c>
       <c r="X440">
         <v>71</v>
       </c>
@@ -89881,6 +91296,36 @@
       <c r="J441" s="12">
         <v>760622</v>
       </c>
+      <c r="K441" t="s">
+        <v>53</v>
+      </c>
+      <c r="L441" t="s">
+        <v>32</v>
+      </c>
+      <c r="M441" t="s">
+        <v>2556</v>
+      </c>
+      <c r="N441" t="s">
+        <v>2557</v>
+      </c>
+      <c r="O441">
+        <v>521</v>
+      </c>
+      <c r="P441">
+        <v>12.2</v>
+      </c>
+      <c r="S441" s="3">
+        <v>42079</v>
+      </c>
+      <c r="U441" t="s">
+        <v>32</v>
+      </c>
+      <c r="V441" t="s">
+        <v>60</v>
+      </c>
+      <c r="W441" t="s">
+        <v>34</v>
+      </c>
       <c r="X441">
         <v>31</v>
       </c>
@@ -89928,6 +91373,9 @@
       <c r="J442" s="12">
         <v>136374</v>
       </c>
+      <c r="R442" t="s">
+        <v>2484</v>
+      </c>
       <c r="X442">
         <v>57</v>
       </c>
@@ -89975,6 +91423,9 @@
       <c r="J443" s="12">
         <v>236904</v>
       </c>
+      <c r="R443" t="s">
+        <v>2484</v>
+      </c>
       <c r="X443">
         <v>50</v>
       </c>
@@ -90022,6 +91473,36 @@
       <c r="J444" s="12">
         <v>300052288</v>
       </c>
+      <c r="K444" t="s">
+        <v>53</v>
+      </c>
+      <c r="L444" t="s">
+        <v>40</v>
+      </c>
+      <c r="M444" t="s">
+        <v>2558</v>
+      </c>
+      <c r="N444" t="s">
+        <v>2559</v>
+      </c>
+      <c r="O444">
+        <v>850</v>
+      </c>
+      <c r="P444">
+        <v>14.1</v>
+      </c>
+      <c r="S444" s="3">
+        <v>42979</v>
+      </c>
+      <c r="U444" t="s">
+        <v>40</v>
+      </c>
+      <c r="V444" t="s">
+        <v>96</v>
+      </c>
+      <c r="W444" t="s">
+        <v>34</v>
+      </c>
       <c r="X444">
         <v>27</v>
       </c>
@@ -90069,6 +91550,9 @@
       <c r="J445" s="12">
         <v>326620</v>
       </c>
+      <c r="R445" t="s">
+        <v>2484</v>
+      </c>
       <c r="X445">
         <v>35</v>
       </c>
@@ -90116,6 +91600,9 @@
       <c r="J446" s="12">
         <v>334164</v>
       </c>
+      <c r="R446" t="s">
+        <v>2484</v>
+      </c>
       <c r="X446">
         <v>59</v>
       </c>
@@ -90163,6 +91650,24 @@
       <c r="J447" s="12">
         <v>455500</v>
       </c>
+      <c r="K447" t="s">
+        <v>30</v>
+      </c>
+      <c r="L447" t="s">
+        <v>154</v>
+      </c>
+      <c r="S447" s="3">
+        <v>38687</v>
+      </c>
+      <c r="T447" s="3">
+        <v>38707</v>
+      </c>
+      <c r="V447" t="s">
+        <v>60</v>
+      </c>
+      <c r="W447" t="s">
+        <v>34</v>
+      </c>
       <c r="X447">
         <v>52</v>
       </c>
@@ -90210,6 +91715,39 @@
       <c r="J448" s="12">
         <v>298149</v>
       </c>
+      <c r="K448" t="s">
+        <v>53</v>
+      </c>
+      <c r="L448" t="s">
+        <v>40</v>
+      </c>
+      <c r="M448" t="s">
+        <v>2560</v>
+      </c>
+      <c r="N448" t="s">
+        <v>2561</v>
+      </c>
+      <c r="O448">
+        <v>683</v>
+      </c>
+      <c r="P448">
+        <v>12.8</v>
+      </c>
+      <c r="Q448" t="s">
+        <v>2562</v>
+      </c>
+      <c r="S448" s="3">
+        <v>42541</v>
+      </c>
+      <c r="U448" t="s">
+        <v>40</v>
+      </c>
+      <c r="V448" t="s">
+        <v>60</v>
+      </c>
+      <c r="W448" t="s">
+        <v>34</v>
+      </c>
       <c r="X448">
         <v>33</v>
       </c>
@@ -90257,6 +91795,39 @@
       <c r="J449" s="12">
         <v>677044</v>
       </c>
+      <c r="K449" t="s">
+        <v>53</v>
+      </c>
+      <c r="L449" t="s">
+        <v>40</v>
+      </c>
+      <c r="M449" t="s">
+        <v>2563</v>
+      </c>
+      <c r="N449" t="s">
+        <v>2564</v>
+      </c>
+      <c r="O449">
+        <v>662</v>
+      </c>
+      <c r="P449">
+        <v>11.4</v>
+      </c>
+      <c r="Q449" t="s">
+        <v>2565</v>
+      </c>
+      <c r="S449" s="3">
+        <v>41278</v>
+      </c>
+      <c r="U449" t="s">
+        <v>40</v>
+      </c>
+      <c r="V449" t="s">
+        <v>60</v>
+      </c>
+      <c r="W449" t="s">
+        <v>34</v>
+      </c>
       <c r="X449">
         <v>24</v>
       </c>
@@ -90304,6 +91875,9 @@
       <c r="J450" s="12">
         <v>731872</v>
       </c>
+      <c r="R450" t="s">
+        <v>2484</v>
+      </c>
       <c r="X450">
         <v>53</v>
       </c>
@@ -90351,6 +91925,30 @@
       <c r="J451" s="12">
         <v>678592</v>
       </c>
+      <c r="K451" t="s">
+        <v>53</v>
+      </c>
+      <c r="L451" t="s">
+        <v>117</v>
+      </c>
+      <c r="M451" t="s">
+        <v>2566</v>
+      </c>
+      <c r="R451" t="s">
+        <v>2567</v>
+      </c>
+      <c r="S451" s="3">
+        <v>40179</v>
+      </c>
+      <c r="U451" t="s">
+        <v>40</v>
+      </c>
+      <c r="V451" t="s">
+        <v>60</v>
+      </c>
+      <c r="W451" t="s">
+        <v>34</v>
+      </c>
       <c r="X451">
         <v>51</v>
       </c>
@@ -90398,6 +91996,15 @@
       <c r="J452" s="12">
         <v>300103380</v>
       </c>
+      <c r="K452" t="s">
+        <v>2465</v>
+      </c>
+      <c r="V452" t="s">
+        <v>2529</v>
+      </c>
+      <c r="W452" t="s">
+        <v>2529</v>
+      </c>
       <c r="X452">
         <v>34</v>
       </c>
@@ -90445,6 +92052,15 @@
       <c r="J453" s="12">
         <v>300104265</v>
       </c>
+      <c r="K453" t="s">
+        <v>2465</v>
+      </c>
+      <c r="V453" t="s">
+        <v>2529</v>
+      </c>
+      <c r="W453" t="s">
+        <v>2529</v>
+      </c>
       <c r="X453">
         <v>58</v>
       </c>
@@ -90492,6 +92108,27 @@
       <c r="J454" s="12">
         <v>662750</v>
       </c>
+      <c r="K454" t="s">
+        <v>30</v>
+      </c>
+      <c r="L454" t="s">
+        <v>2568</v>
+      </c>
+      <c r="S454" s="3">
+        <v>41367</v>
+      </c>
+      <c r="T454" s="3">
+        <v>41372</v>
+      </c>
+      <c r="U454" t="s">
+        <v>2569</v>
+      </c>
+      <c r="V454" t="s">
+        <v>2570</v>
+      </c>
+      <c r="W454" t="s">
+        <v>34</v>
+      </c>
       <c r="X454">
         <v>67</v>
       </c>
@@ -90539,6 +92176,21 @@
       <c r="J455" s="12">
         <v>470993</v>
       </c>
+      <c r="K455" t="s">
+        <v>2465</v>
+      </c>
+      <c r="L455" t="s">
+        <v>40</v>
+      </c>
+      <c r="M455" t="s">
+        <v>2571</v>
+      </c>
+      <c r="V455" t="s">
+        <v>2529</v>
+      </c>
+      <c r="W455" t="s">
+        <v>2529</v>
+      </c>
       <c r="X455">
         <v>31</v>
       </c>
@@ -90586,6 +92238,39 @@
       <c r="J456" s="12">
         <v>662362</v>
       </c>
+      <c r="K456" t="s">
+        <v>30</v>
+      </c>
+      <c r="L456" t="s">
+        <v>32</v>
+      </c>
+      <c r="M456" t="s">
+        <v>2572</v>
+      </c>
+      <c r="N456" t="s">
+        <v>2573</v>
+      </c>
+      <c r="O456">
+        <v>673</v>
+      </c>
+      <c r="P456">
+        <v>13.5</v>
+      </c>
+      <c r="Q456" t="s">
+        <v>2574</v>
+      </c>
+      <c r="S456" s="3">
+        <v>41518</v>
+      </c>
+      <c r="U456" t="s">
+        <v>40</v>
+      </c>
+      <c r="V456" t="s">
+        <v>157</v>
+      </c>
+      <c r="W456" t="s">
+        <v>157</v>
+      </c>
       <c r="X456">
         <v>40</v>
       </c>
@@ -90633,6 +92318,24 @@
       <c r="J457" s="12">
         <v>512319</v>
       </c>
+      <c r="K457" t="s">
+        <v>53</v>
+      </c>
+      <c r="L457" t="s">
+        <v>40</v>
+      </c>
+      <c r="S457" s="3">
+        <v>39630</v>
+      </c>
+      <c r="U457" t="s">
+        <v>40</v>
+      </c>
+      <c r="V457" t="s">
+        <v>60</v>
+      </c>
+      <c r="W457" t="s">
+        <v>34</v>
+      </c>
       <c r="X457">
         <v>51</v>
       </c>
@@ -90680,6 +92383,9 @@
       <c r="J458" s="12">
         <v>300054363</v>
       </c>
+      <c r="R458" t="s">
+        <v>2484</v>
+      </c>
       <c r="X458">
         <v>50</v>
       </c>
@@ -90727,6 +92433,36 @@
       <c r="J459" s="12">
         <v>300044383</v>
       </c>
+      <c r="K459" t="s">
+        <v>30</v>
+      </c>
+      <c r="L459" t="s">
+        <v>32</v>
+      </c>
+      <c r="M459" t="s">
+        <v>2575</v>
+      </c>
+      <c r="N459" t="s">
+        <v>2576</v>
+      </c>
+      <c r="O459">
+        <v>825</v>
+      </c>
+      <c r="P459">
+        <v>11.7</v>
+      </c>
+      <c r="S459" s="3">
+        <v>42705</v>
+      </c>
+      <c r="U459" t="s">
+        <v>40</v>
+      </c>
+      <c r="V459" t="s">
+        <v>157</v>
+      </c>
+      <c r="W459" t="s">
+        <v>157</v>
+      </c>
       <c r="X459">
         <v>23</v>
       </c>
@@ -90774,6 +92510,27 @@
       <c r="J460" s="12">
         <v>724566</v>
       </c>
+      <c r="K460" t="s">
+        <v>30</v>
+      </c>
+      <c r="L460" t="s">
+        <v>120</v>
+      </c>
+      <c r="S460" s="3">
+        <v>43191</v>
+      </c>
+      <c r="T460" s="3">
+        <v>43238</v>
+      </c>
+      <c r="U460" t="s">
+        <v>2568</v>
+      </c>
+      <c r="V460" t="s">
+        <v>33</v>
+      </c>
+      <c r="W460" t="s">
+        <v>34</v>
+      </c>
       <c r="X460">
         <v>80</v>
       </c>
@@ -90821,6 +92578,39 @@
       <c r="J461" s="12">
         <v>635720</v>
       </c>
+      <c r="K461" t="s">
+        <v>30</v>
+      </c>
+      <c r="L461" t="s">
+        <v>32</v>
+      </c>
+      <c r="M461" t="s">
+        <v>2577</v>
+      </c>
+      <c r="N461" t="s">
+        <v>2578</v>
+      </c>
+      <c r="O461">
+        <v>550</v>
+      </c>
+      <c r="P461">
+        <v>15</v>
+      </c>
+      <c r="S461" s="3">
+        <v>40856</v>
+      </c>
+      <c r="T461" s="3">
+        <v>40924</v>
+      </c>
+      <c r="U461" t="s">
+        <v>40</v>
+      </c>
+      <c r="V461" t="s">
+        <v>157</v>
+      </c>
+      <c r="W461" t="s">
+        <v>157</v>
+      </c>
       <c r="X461">
         <v>40</v>
       </c>
@@ -90915,6 +92705,18 @@
       <c r="J463" s="12">
         <v>302788</v>
       </c>
+      <c r="K463" t="s">
+        <v>2465</v>
+      </c>
+      <c r="S463" s="3">
+        <v>43206</v>
+      </c>
+      <c r="V463" t="s">
+        <v>2529</v>
+      </c>
+      <c r="W463" t="s">
+        <v>2529</v>
+      </c>
       <c r="X463">
         <v>50</v>
       </c>
@@ -90962,6 +92764,36 @@
       <c r="J464" s="12">
         <v>82016</v>
       </c>
+      <c r="K464" t="s">
+        <v>53</v>
+      </c>
+      <c r="L464" t="s">
+        <v>117</v>
+      </c>
+      <c r="M464" t="s">
+        <v>2579</v>
+      </c>
+      <c r="N464" t="s">
+        <v>2580</v>
+      </c>
+      <c r="O464">
+        <v>707</v>
+      </c>
+      <c r="P464">
+        <v>14.1</v>
+      </c>
+      <c r="S464" s="3">
+        <v>42943</v>
+      </c>
+      <c r="U464" t="s">
+        <v>40</v>
+      </c>
+      <c r="V464" t="s">
+        <v>96</v>
+      </c>
+      <c r="W464" t="s">
+        <v>34</v>
+      </c>
       <c r="X464">
         <v>51</v>
       </c>
@@ -91009,6 +92841,9 @@
       <c r="J465" s="12">
         <v>703116</v>
       </c>
+      <c r="R465" t="s">
+        <v>2484</v>
+      </c>
       <c r="X465">
         <v>28</v>
       </c>
@@ -91056,6 +92891,27 @@
       <c r="J466" s="12">
         <v>157875</v>
       </c>
+      <c r="K466" t="s">
+        <v>30</v>
+      </c>
+      <c r="L466" t="s">
+        <v>2581</v>
+      </c>
+      <c r="S466" s="3">
+        <v>38443</v>
+      </c>
+      <c r="T466" s="3">
+        <v>38456</v>
+      </c>
+      <c r="U466" t="s">
+        <v>2513</v>
+      </c>
+      <c r="V466" t="s">
+        <v>60</v>
+      </c>
+      <c r="W466" t="s">
+        <v>34</v>
+      </c>
       <c r="X466">
         <v>80</v>
       </c>
@@ -91103,6 +92959,15 @@
       <c r="J467" s="12">
         <v>622312</v>
       </c>
+      <c r="K467" t="s">
+        <v>2465</v>
+      </c>
+      <c r="V467" t="s">
+        <v>2529</v>
+      </c>
+      <c r="W467" s="9" t="s">
+        <v>2529</v>
+      </c>
       <c r="X467">
         <v>25</v>
       </c>
@@ -91150,6 +93015,24 @@
       <c r="J468" s="12">
         <v>593992</v>
       </c>
+      <c r="K468" t="s">
+        <v>53</v>
+      </c>
+      <c r="L468" t="s">
+        <v>32</v>
+      </c>
+      <c r="S468" s="3">
+        <v>41426</v>
+      </c>
+      <c r="U468" t="s">
+        <v>40</v>
+      </c>
+      <c r="V468" t="s">
+        <v>157</v>
+      </c>
+      <c r="W468" t="s">
+        <v>157</v>
+      </c>
       <c r="X468">
         <v>48</v>
       </c>
@@ -91197,6 +93080,36 @@
       <c r="J469" s="12">
         <v>570064</v>
       </c>
+      <c r="K469" t="s">
+        <v>30</v>
+      </c>
+      <c r="L469" t="s">
+        <v>40</v>
+      </c>
+      <c r="M469">
+        <v>6.5</v>
+      </c>
+      <c r="N469" t="s">
+        <v>2582</v>
+      </c>
+      <c r="R469" t="s">
+        <v>2583</v>
+      </c>
+      <c r="S469" s="3">
+        <v>40087</v>
+      </c>
+      <c r="T469" s="3">
+        <v>40119</v>
+      </c>
+      <c r="U469" t="s">
+        <v>40</v>
+      </c>
+      <c r="V469" t="s">
+        <v>60</v>
+      </c>
+      <c r="W469" t="s">
+        <v>34</v>
+      </c>
       <c r="X469">
         <v>52</v>
       </c>
@@ -91244,6 +93157,36 @@
       <c r="J470" s="12">
         <v>404252</v>
       </c>
+      <c r="K470" t="s">
+        <v>53</v>
+      </c>
+      <c r="L470" t="s">
+        <v>117</v>
+      </c>
+      <c r="M470">
+        <v>7.4</v>
+      </c>
+      <c r="N470" t="s">
+        <v>2584</v>
+      </c>
+      <c r="O470">
+        <v>588</v>
+      </c>
+      <c r="P470">
+        <v>23.3</v>
+      </c>
+      <c r="S470" s="3">
+        <v>41978</v>
+      </c>
+      <c r="U470" t="s">
+        <v>40</v>
+      </c>
+      <c r="V470" t="s">
+        <v>96</v>
+      </c>
+      <c r="W470" t="s">
+        <v>34</v>
+      </c>
       <c r="X470">
         <v>75</v>
       </c>
@@ -91291,6 +93234,39 @@
       <c r="J471" s="12">
         <v>562753</v>
       </c>
+      <c r="K471" t="s">
+        <v>53</v>
+      </c>
+      <c r="L471" t="s">
+        <v>40</v>
+      </c>
+      <c r="M471">
+        <v>15</v>
+      </c>
+      <c r="N471" t="s">
+        <v>2585</v>
+      </c>
+      <c r="O471">
+        <v>704</v>
+      </c>
+      <c r="P471">
+        <v>13</v>
+      </c>
+      <c r="Q471" t="s">
+        <v>2586</v>
+      </c>
+      <c r="S471" s="3">
+        <v>41870</v>
+      </c>
+      <c r="U471" t="s">
+        <v>40</v>
+      </c>
+      <c r="V471" t="s">
+        <v>96</v>
+      </c>
+      <c r="W471" t="s">
+        <v>34</v>
+      </c>
       <c r="X471">
         <v>47</v>
       </c>
@@ -91338,6 +93314,18 @@
       <c r="J472" s="12">
         <v>300014983</v>
       </c>
+      <c r="K472" t="s">
+        <v>2465</v>
+      </c>
+      <c r="S472" s="3">
+        <v>43169</v>
+      </c>
+      <c r="V472" t="s">
+        <v>2529</v>
+      </c>
+      <c r="W472" s="9" t="s">
+        <v>2529</v>
+      </c>
       <c r="X472">
         <v>35</v>
       </c>
@@ -91385,6 +93373,9 @@
       <c r="J473" s="12">
         <v>705118</v>
       </c>
+      <c r="R473" t="s">
+        <v>2484</v>
+      </c>
       <c r="X473">
         <v>56</v>
       </c>
@@ -91432,6 +93423,24 @@
       <c r="J474" s="12">
         <v>659263</v>
       </c>
+      <c r="K474" t="s">
+        <v>53</v>
+      </c>
+      <c r="L474" t="s">
+        <v>212</v>
+      </c>
+      <c r="S474" s="3">
+        <v>40951</v>
+      </c>
+      <c r="U474" t="s">
+        <v>40</v>
+      </c>
+      <c r="V474" t="s">
+        <v>96</v>
+      </c>
+      <c r="W474" t="s">
+        <v>34</v>
+      </c>
       <c r="X474">
         <v>30</v>
       </c>
@@ -91479,6 +93488,24 @@
       <c r="J475" s="12">
         <v>166990</v>
       </c>
+      <c r="K475" t="s">
+        <v>53</v>
+      </c>
+      <c r="L475" t="s">
+        <v>117</v>
+      </c>
+      <c r="S475" s="3">
+        <v>42955</v>
+      </c>
+      <c r="U475" t="s">
+        <v>40</v>
+      </c>
+      <c r="V475" t="s">
+        <v>60</v>
+      </c>
+      <c r="W475" t="s">
+        <v>34</v>
+      </c>
       <c r="X475">
         <v>34</v>
       </c>
@@ -91526,6 +93553,24 @@
       <c r="J476" s="12">
         <v>268594</v>
       </c>
+      <c r="K476" t="s">
+        <v>30</v>
+      </c>
+      <c r="L476" t="s">
+        <v>112</v>
+      </c>
+      <c r="S476" s="3">
+        <v>43137</v>
+      </c>
+      <c r="U476" t="s">
+        <v>112</v>
+      </c>
+      <c r="V476" t="s">
+        <v>96</v>
+      </c>
+      <c r="W476" t="s">
+        <v>34</v>
+      </c>
       <c r="X476">
         <v>77</v>
       </c>
@@ -91573,6 +93618,27 @@
       <c r="J477" s="12">
         <v>121913</v>
       </c>
+      <c r="K477" t="s">
+        <v>30</v>
+      </c>
+      <c r="L477" t="s">
+        <v>40</v>
+      </c>
+      <c r="S477" s="3">
+        <v>42782</v>
+      </c>
+      <c r="T477" s="3">
+        <v>42793</v>
+      </c>
+      <c r="U477" t="s">
+        <v>40</v>
+      </c>
+      <c r="V477" t="s">
+        <v>96</v>
+      </c>
+      <c r="W477" t="s">
+        <v>34</v>
+      </c>
       <c r="X477">
         <v>54</v>
       </c>
@@ -91620,6 +93686,24 @@
       <c r="J478" s="12">
         <v>305664</v>
       </c>
+      <c r="K478" t="s">
+        <v>30</v>
+      </c>
+      <c r="L478" t="s">
+        <v>32</v>
+      </c>
+      <c r="S478" s="3">
+        <v>40969</v>
+      </c>
+      <c r="U478" t="s">
+        <v>40</v>
+      </c>
+      <c r="V478" t="s">
+        <v>157</v>
+      </c>
+      <c r="W478" t="s">
+        <v>157</v>
+      </c>
       <c r="X478">
         <v>59</v>
       </c>
@@ -91667,6 +93751,27 @@
       <c r="J479" s="12">
         <v>493633</v>
       </c>
+      <c r="K479" t="s">
+        <v>30</v>
+      </c>
+      <c r="L479" t="s">
+        <v>117</v>
+      </c>
+      <c r="S479" s="3">
+        <v>39052</v>
+      </c>
+      <c r="T479" s="3">
+        <v>39587</v>
+      </c>
+      <c r="U479" t="s">
+        <v>40</v>
+      </c>
+      <c r="V479" t="s">
+        <v>60</v>
+      </c>
+      <c r="W479" t="s">
+        <v>34</v>
+      </c>
       <c r="X479">
         <v>32</v>
       </c>
@@ -91714,6 +93819,18 @@
       <c r="J480" s="12">
         <v>23613</v>
       </c>
+      <c r="K480" t="s">
+        <v>2465</v>
+      </c>
+      <c r="U480" t="s">
+        <v>40</v>
+      </c>
+      <c r="V480" t="s">
+        <v>2529</v>
+      </c>
+      <c r="W480" s="9" t="s">
+        <v>2529</v>
+      </c>
       <c r="X480">
         <v>46</v>
       </c>
@@ -91761,6 +93878,21 @@
       <c r="J481" s="12">
         <v>300089704</v>
       </c>
+      <c r="K481" t="s">
+        <v>2465</v>
+      </c>
+      <c r="S481" s="3">
+        <v>43125</v>
+      </c>
+      <c r="U481" t="s">
+        <v>40</v>
+      </c>
+      <c r="V481" t="s">
+        <v>2529</v>
+      </c>
+      <c r="W481" s="9" t="s">
+        <v>2529</v>
+      </c>
       <c r="X481">
         <v>26</v>
       </c>
@@ -91808,6 +93940,24 @@
       <c r="J482" s="12">
         <v>430196</v>
       </c>
+      <c r="K482" t="s">
+        <v>53</v>
+      </c>
+      <c r="L482" t="s">
+        <v>32</v>
+      </c>
+      <c r="S482" s="3">
+        <v>43119</v>
+      </c>
+      <c r="U482" t="s">
+        <v>40</v>
+      </c>
+      <c r="V482" t="s">
+        <v>157</v>
+      </c>
+      <c r="W482" t="s">
+        <v>157</v>
+      </c>
       <c r="X482">
         <v>57</v>
       </c>
@@ -91855,6 +94005,45 @@
       <c r="J483" s="12">
         <v>300071920</v>
       </c>
+      <c r="K483" t="s">
+        <v>53</v>
+      </c>
+      <c r="L483" t="s">
+        <v>117</v>
+      </c>
+      <c r="M483" t="s">
+        <v>2587</v>
+      </c>
+      <c r="N483" t="s">
+        <v>2588</v>
+      </c>
+      <c r="O483">
+        <v>1150</v>
+      </c>
+      <c r="P483" s="6">
+        <v>11.8</v>
+      </c>
+      <c r="Q483" t="s">
+        <v>2589</v>
+      </c>
+      <c r="R483" t="s">
+        <v>2590</v>
+      </c>
+      <c r="S483" s="3">
+        <v>42917</v>
+      </c>
+      <c r="T483" s="3">
+        <v>42984</v>
+      </c>
+      <c r="U483" t="s">
+        <v>40</v>
+      </c>
+      <c r="V483" t="s">
+        <v>55</v>
+      </c>
+      <c r="W483" t="s">
+        <v>34</v>
+      </c>
       <c r="X483">
         <v>57</v>
       </c>
@@ -91902,6 +94091,24 @@
       <c r="J484" s="12">
         <v>719666</v>
       </c>
+      <c r="K484" t="s">
+        <v>30</v>
+      </c>
+      <c r="L484" t="s">
+        <v>164</v>
+      </c>
+      <c r="S484" s="3">
+        <v>41699</v>
+      </c>
+      <c r="U484" t="s">
+        <v>164</v>
+      </c>
+      <c r="V484" t="s">
+        <v>157</v>
+      </c>
+      <c r="W484" t="s">
+        <v>157</v>
+      </c>
       <c r="X484">
         <v>70</v>
       </c>
@@ -91949,6 +94156,9 @@
       <c r="J485" s="12">
         <v>300060205</v>
       </c>
+      <c r="R485" t="s">
+        <v>2484</v>
+      </c>
       <c r="X485">
         <v>43</v>
       </c>
@@ -91996,6 +94206,18 @@
       <c r="J486" s="12">
         <v>187431</v>
       </c>
+      <c r="K486" t="s">
+        <v>2465</v>
+      </c>
+      <c r="S486" s="3">
+        <v>43052</v>
+      </c>
+      <c r="V486" t="s">
+        <v>2529</v>
+      </c>
+      <c r="W486" s="9" t="s">
+        <v>2529</v>
+      </c>
       <c r="X486">
         <v>56</v>
       </c>
@@ -92043,6 +94265,24 @@
       <c r="J487" s="12">
         <v>300005306</v>
       </c>
+      <c r="K487" t="s">
+        <v>53</v>
+      </c>
+      <c r="L487" t="s">
+        <v>40</v>
+      </c>
+      <c r="R487" t="s">
+        <v>2591</v>
+      </c>
+      <c r="S487" s="3">
+        <v>43040</v>
+      </c>
+      <c r="V487" t="s">
+        <v>96</v>
+      </c>
+      <c r="W487" t="s">
+        <v>34</v>
+      </c>
       <c r="X487">
         <v>39</v>
       </c>
@@ -92090,6 +94330,9 @@
       <c r="J488" s="12">
         <v>300074797</v>
       </c>
+      <c r="R488" t="s">
+        <v>2484</v>
+      </c>
       <c r="X488">
         <v>50</v>
       </c>
@@ -92137,6 +94380,18 @@
       <c r="J489" s="12">
         <v>676149</v>
       </c>
+      <c r="K489" t="s">
+        <v>2465</v>
+      </c>
+      <c r="U489" t="s">
+        <v>40</v>
+      </c>
+      <c r="V489" t="s">
+        <v>2529</v>
+      </c>
+      <c r="W489" s="9" t="s">
+        <v>2529</v>
+      </c>
       <c r="X489">
         <v>54</v>
       </c>
@@ -92184,6 +94439,24 @@
       <c r="J490" s="12">
         <v>393986</v>
       </c>
+      <c r="K490" t="s">
+        <v>53</v>
+      </c>
+      <c r="L490" t="s">
+        <v>40</v>
+      </c>
+      <c r="S490" s="3">
+        <v>39722</v>
+      </c>
+      <c r="U490" t="s">
+        <v>40</v>
+      </c>
+      <c r="V490" t="s">
+        <v>96</v>
+      </c>
+      <c r="W490" t="s">
+        <v>34</v>
+      </c>
       <c r="X490">
         <v>50</v>
       </c>
@@ -92231,6 +94504,30 @@
       <c r="J491" s="12">
         <v>300076492</v>
       </c>
+      <c r="K491" t="s">
+        <v>30</v>
+      </c>
+      <c r="L491" t="s">
+        <v>32</v>
+      </c>
+      <c r="R491" t="s">
+        <v>2592</v>
+      </c>
+      <c r="S491" s="3">
+        <v>42600</v>
+      </c>
+      <c r="T491" s="3">
+        <v>42996</v>
+      </c>
+      <c r="U491" t="s">
+        <v>2593</v>
+      </c>
+      <c r="V491" t="s">
+        <v>157</v>
+      </c>
+      <c r="W491" t="s">
+        <v>157</v>
+      </c>
       <c r="X491">
         <v>60</v>
       </c>
@@ -92278,6 +94575,24 @@
       <c r="J492" s="12">
         <v>14433</v>
       </c>
+      <c r="K492" t="s">
+        <v>53</v>
+      </c>
+      <c r="L492" t="s">
+        <v>40</v>
+      </c>
+      <c r="S492" s="3">
+        <v>42552</v>
+      </c>
+      <c r="U492" t="s">
+        <v>40</v>
+      </c>
+      <c r="V492" t="s">
+        <v>60</v>
+      </c>
+      <c r="W492" t="s">
+        <v>34</v>
+      </c>
       <c r="X492">
         <v>77</v>
       </c>
@@ -92325,6 +94640,24 @@
       <c r="J493" s="12">
         <v>563268</v>
       </c>
+      <c r="K493" t="s">
+        <v>30</v>
+      </c>
+      <c r="L493" t="s">
+        <v>32</v>
+      </c>
+      <c r="S493" s="3">
+        <v>40026</v>
+      </c>
+      <c r="U493" t="s">
+        <v>40</v>
+      </c>
+      <c r="V493" t="s">
+        <v>157</v>
+      </c>
+      <c r="W493" t="s">
+        <v>157</v>
+      </c>
       <c r="X493">
         <v>85</v>
       </c>
@@ -92372,6 +94705,24 @@
       <c r="J494" s="12">
         <v>771570</v>
       </c>
+      <c r="K494" t="s">
+        <v>53</v>
+      </c>
+      <c r="L494" t="s">
+        <v>32</v>
+      </c>
+      <c r="S494" s="3">
+        <v>41671</v>
+      </c>
+      <c r="U494" t="s">
+        <v>40</v>
+      </c>
+      <c r="V494" t="s">
+        <v>157</v>
+      </c>
+      <c r="W494" t="s">
+        <v>157</v>
+      </c>
       <c r="X494">
         <v>31</v>
       </c>
@@ -92419,6 +94770,9 @@
       <c r="J495" s="12">
         <v>347729</v>
       </c>
+      <c r="R495" t="s">
+        <v>2484</v>
+      </c>
       <c r="X495">
         <v>78</v>
       </c>
@@ -92466,6 +94820,9 @@
       <c r="J496" s="12">
         <v>601199</v>
       </c>
+      <c r="R496" t="s">
+        <v>2484</v>
+      </c>
       <c r="X496">
         <v>50</v>
       </c>
@@ -92513,6 +94870,27 @@
       <c r="J497" s="12">
         <v>300038846</v>
       </c>
+      <c r="K497" t="s">
+        <v>53</v>
+      </c>
+      <c r="L497" t="s">
+        <v>117</v>
+      </c>
+      <c r="S497" s="3">
+        <v>42677</v>
+      </c>
+      <c r="T497" s="16">
+        <v>42816</v>
+      </c>
+      <c r="U497" t="s">
+        <v>40</v>
+      </c>
+      <c r="V497" t="s">
+        <v>42</v>
+      </c>
+      <c r="W497" t="s">
+        <v>34</v>
+      </c>
       <c r="X497">
         <v>55</v>
       </c>
@@ -92560,6 +94938,27 @@
       <c r="J498" s="12">
         <v>224630</v>
       </c>
+      <c r="K498" t="s">
+        <v>53</v>
+      </c>
+      <c r="L498" t="s">
+        <v>117</v>
+      </c>
+      <c r="S498" s="3">
+        <v>42644</v>
+      </c>
+      <c r="T498" s="3">
+        <v>42809</v>
+      </c>
+      <c r="U498" t="s">
+        <v>40</v>
+      </c>
+      <c r="V498" t="s">
+        <v>42</v>
+      </c>
+      <c r="W498" t="s">
+        <v>34</v>
+      </c>
       <c r="X498">
         <v>62</v>
       </c>
@@ -92607,6 +95006,21 @@
       <c r="J499" s="12">
         <v>538377</v>
       </c>
+      <c r="K499" t="s">
+        <v>2465</v>
+      </c>
+      <c r="L499" t="s">
+        <v>40</v>
+      </c>
+      <c r="U499" t="s">
+        <v>40</v>
+      </c>
+      <c r="V499" t="s">
+        <v>2529</v>
+      </c>
+      <c r="W499" s="9" t="s">
+        <v>2529</v>
+      </c>
       <c r="X499">
         <v>25</v>
       </c>
@@ -92654,6 +95068,30 @@
       <c r="J500" s="12">
         <v>631872</v>
       </c>
+      <c r="K500" t="s">
+        <v>30</v>
+      </c>
+      <c r="L500" t="s">
+        <v>2594</v>
+      </c>
+      <c r="R500" t="s">
+        <v>2595</v>
+      </c>
+      <c r="S500" s="3">
+        <v>40848</v>
+      </c>
+      <c r="T500" s="3">
+        <v>40854</v>
+      </c>
+      <c r="U500" t="s">
+        <v>32</v>
+      </c>
+      <c r="V500" t="s">
+        <v>33</v>
+      </c>
+      <c r="W500" t="s">
+        <v>34</v>
+      </c>
       <c r="X500">
         <v>82</v>
       </c>
@@ -92701,6 +95139,27 @@
       <c r="J501" s="12">
         <v>89316</v>
       </c>
+      <c r="K501" t="s">
+        <v>30</v>
+      </c>
+      <c r="L501" t="s">
+        <v>2593</v>
+      </c>
+      <c r="S501" s="3">
+        <v>33604</v>
+      </c>
+      <c r="T501" s="3">
+        <v>33604</v>
+      </c>
+      <c r="U501" t="s">
+        <v>2593</v>
+      </c>
+      <c r="V501" t="s">
+        <v>60</v>
+      </c>
+      <c r="W501" t="s">
+        <v>34</v>
+      </c>
       <c r="X501">
         <v>50</v>
       </c>
@@ -92748,6 +95207,21 @@
       <c r="J502" s="12">
         <v>640481</v>
       </c>
+      <c r="K502" t="s">
+        <v>2465</v>
+      </c>
+      <c r="L502" t="s">
+        <v>117</v>
+      </c>
+      <c r="U502" t="s">
+        <v>40</v>
+      </c>
+      <c r="V502" t="s">
+        <v>2529</v>
+      </c>
+      <c r="W502" s="9" t="s">
+        <v>2529</v>
+      </c>
       <c r="X502">
         <v>34</v>
       </c>
@@ -92795,6 +95269,9 @@
       <c r="J503" s="12">
         <v>235789</v>
       </c>
+      <c r="R503" t="s">
+        <v>2484</v>
+      </c>
       <c r="X503">
         <v>68</v>
       </c>
@@ -92842,6 +95319,24 @@
       <c r="J504" s="12">
         <v>79730</v>
       </c>
+      <c r="K504" t="s">
+        <v>53</v>
+      </c>
+      <c r="L504" t="s">
+        <v>117</v>
+      </c>
+      <c r="S504" s="3">
+        <v>41208</v>
+      </c>
+      <c r="U504" t="s">
+        <v>40</v>
+      </c>
+      <c r="V504" t="s">
+        <v>60</v>
+      </c>
+      <c r="W504" t="s">
+        <v>34</v>
+      </c>
       <c r="X504">
         <v>29</v>
       </c>
@@ -92889,6 +95384,9 @@
       <c r="J505" s="12">
         <v>600064</v>
       </c>
+      <c r="R505" t="s">
+        <v>2484</v>
+      </c>
       <c r="X505">
         <v>58</v>
       </c>
@@ -92936,6 +95434,9 @@
       <c r="J506" s="12">
         <v>277820</v>
       </c>
+      <c r="R506" t="s">
+        <v>2484</v>
+      </c>
       <c r="X506">
         <v>63</v>
       </c>
@@ -92983,6 +95484,24 @@
       <c r="J507" s="12">
         <v>427032</v>
       </c>
+      <c r="K507" t="s">
+        <v>53</v>
+      </c>
+      <c r="L507" t="s">
+        <v>40</v>
+      </c>
+      <c r="S507" s="3">
+        <v>41570</v>
+      </c>
+      <c r="U507" t="s">
+        <v>40</v>
+      </c>
+      <c r="V507" t="s">
+        <v>42</v>
+      </c>
+      <c r="W507" t="s">
+        <v>34</v>
+      </c>
       <c r="X507">
         <v>72</v>
       </c>
@@ -93030,6 +95549,9 @@
       <c r="J508" s="12">
         <v>123491</v>
       </c>
+      <c r="R508" t="s">
+        <v>2484</v>
+      </c>
       <c r="X508">
         <v>52</v>
       </c>
@@ -93077,6 +95599,9 @@
       <c r="J509" s="12">
         <v>477526</v>
       </c>
+      <c r="R509" t="s">
+        <v>2484</v>
+      </c>
       <c r="X509">
         <v>49</v>
       </c>
@@ -93124,6 +95649,27 @@
       <c r="J510" s="12">
         <v>500834</v>
       </c>
+      <c r="K510" t="s">
+        <v>53</v>
+      </c>
+      <c r="L510" t="s">
+        <v>32</v>
+      </c>
+      <c r="S510" s="3">
+        <v>39356</v>
+      </c>
+      <c r="T510" s="3">
+        <v>39370</v>
+      </c>
+      <c r="U510" t="s">
+        <v>40</v>
+      </c>
+      <c r="V510" t="s">
+        <v>157</v>
+      </c>
+      <c r="W510" t="s">
+        <v>157</v>
+      </c>
       <c r="X510">
         <v>34</v>
       </c>
@@ -93171,6 +95717,24 @@
       <c r="J511" s="12">
         <v>523346</v>
       </c>
+      <c r="K511" t="s">
+        <v>30</v>
+      </c>
+      <c r="L511" t="s">
+        <v>32</v>
+      </c>
+      <c r="S511" s="3">
+        <v>39569</v>
+      </c>
+      <c r="U511" t="s">
+        <v>40</v>
+      </c>
+      <c r="V511" t="s">
+        <v>157</v>
+      </c>
+      <c r="W511" t="s">
+        <v>157</v>
+      </c>
       <c r="X511">
         <v>73</v>
       </c>
@@ -93218,6 +95782,24 @@
       <c r="J512" s="12">
         <v>65280</v>
       </c>
+      <c r="K512" t="s">
+        <v>53</v>
+      </c>
+      <c r="L512" t="s">
+        <v>40</v>
+      </c>
+      <c r="S512" s="3">
+        <v>42701</v>
+      </c>
+      <c r="U512" t="s">
+        <v>40</v>
+      </c>
+      <c r="V512" t="s">
+        <v>96</v>
+      </c>
+      <c r="W512" t="s">
+        <v>34</v>
+      </c>
       <c r="X512">
         <v>44</v>
       </c>
@@ -93265,6 +95847,9 @@
       <c r="J513" s="12">
         <v>650215</v>
       </c>
+      <c r="R513" t="s">
+        <v>2484</v>
+      </c>
       <c r="X513">
         <v>25</v>
       </c>
@@ -93312,6 +95897,30 @@
       <c r="J514" s="12">
         <v>485293</v>
       </c>
+      <c r="K514" t="s">
+        <v>30</v>
+      </c>
+      <c r="L514" t="s">
+        <v>2593</v>
+      </c>
+      <c r="R514" t="s">
+        <v>2596</v>
+      </c>
+      <c r="S514" s="3">
+        <v>39087</v>
+      </c>
+      <c r="T514" s="3">
+        <v>39106</v>
+      </c>
+      <c r="U514" s="7" t="s">
+        <v>2593</v>
+      </c>
+      <c r="V514" t="s">
+        <v>60</v>
+      </c>
+      <c r="W514" t="s">
+        <v>34</v>
+      </c>
       <c r="X514">
         <v>78</v>
       </c>
@@ -93359,6 +95968,24 @@
       <c r="J515" s="12">
         <v>756395</v>
       </c>
+      <c r="K515" t="s">
+        <v>53</v>
+      </c>
+      <c r="L515" t="s">
+        <v>32</v>
+      </c>
+      <c r="S515" s="3">
+        <v>41974</v>
+      </c>
+      <c r="U515" t="s">
+        <v>40</v>
+      </c>
+      <c r="V515" t="s">
+        <v>157</v>
+      </c>
+      <c r="W515" t="s">
+        <v>157</v>
+      </c>
       <c r="X515">
         <v>30</v>
       </c>
@@ -93406,6 +96033,9 @@
       <c r="J516" s="12">
         <v>563249</v>
       </c>
+      <c r="R516" t="s">
+        <v>2484</v>
+      </c>
       <c r="X516">
         <v>75</v>
       </c>
@@ -93453,6 +96083,33 @@
       <c r="J517" s="12">
         <v>595661</v>
       </c>
+      <c r="K517" t="s">
+        <v>30</v>
+      </c>
+      <c r="L517" t="s">
+        <v>164</v>
+      </c>
+      <c r="M517" t="s">
+        <v>2555</v>
+      </c>
+      <c r="R517" t="s">
+        <v>2596</v>
+      </c>
+      <c r="S517" s="3">
+        <v>40360</v>
+      </c>
+      <c r="T517" s="3">
+        <v>40387</v>
+      </c>
+      <c r="U517" t="s">
+        <v>41</v>
+      </c>
+      <c r="V517" t="s">
+        <v>157</v>
+      </c>
+      <c r="W517" t="s">
+        <v>157</v>
+      </c>
       <c r="X517">
         <v>30</v>
       </c>
@@ -93500,6 +96157,24 @@
       <c r="J518" s="12">
         <v>86428</v>
       </c>
+      <c r="K518" t="s">
+        <v>53</v>
+      </c>
+      <c r="L518" t="s">
+        <v>117</v>
+      </c>
+      <c r="S518" s="3">
+        <v>41821</v>
+      </c>
+      <c r="U518" t="s">
+        <v>40</v>
+      </c>
+      <c r="V518" t="s">
+        <v>60</v>
+      </c>
+      <c r="W518" t="s">
+        <v>34</v>
+      </c>
       <c r="X518">
         <v>42</v>
       </c>
@@ -93547,6 +96222,9 @@
       <c r="J519" s="12">
         <v>130397</v>
       </c>
+      <c r="R519" t="s">
+        <v>2484</v>
+      </c>
       <c r="X519">
         <v>45</v>
       </c>
@@ -93594,6 +96272,24 @@
       <c r="J520" s="12">
         <v>723521</v>
       </c>
+      <c r="K520" t="s">
+        <v>53</v>
+      </c>
+      <c r="L520" t="s">
+        <v>32</v>
+      </c>
+      <c r="S520" s="3">
+        <v>41730</v>
+      </c>
+      <c r="U520" t="s">
+        <v>40</v>
+      </c>
+      <c r="V520" t="s">
+        <v>157</v>
+      </c>
+      <c r="W520" t="s">
+        <v>157</v>
+      </c>
       <c r="X520">
         <v>29</v>
       </c>
@@ -93641,6 +96337,24 @@
       <c r="J521" s="12">
         <v>306125</v>
       </c>
+      <c r="K521" t="s">
+        <v>53</v>
+      </c>
+      <c r="L521" t="s">
+        <v>32</v>
+      </c>
+      <c r="S521" s="3">
+        <v>41955</v>
+      </c>
+      <c r="U521" t="s">
+        <v>40</v>
+      </c>
+      <c r="V521" t="s">
+        <v>157</v>
+      </c>
+      <c r="W521" t="s">
+        <v>157</v>
+      </c>
       <c r="X521">
         <v>58</v>
       </c>
@@ -93688,6 +96402,24 @@
       <c r="J522" s="12">
         <v>93651</v>
       </c>
+      <c r="K522" t="s">
+        <v>30</v>
+      </c>
+      <c r="L522" t="s">
+        <v>40</v>
+      </c>
+      <c r="S522" s="3">
+        <v>41061</v>
+      </c>
+      <c r="U522" t="s">
+        <v>40</v>
+      </c>
+      <c r="V522" t="s">
+        <v>60</v>
+      </c>
+      <c r="W522" t="s">
+        <v>34</v>
+      </c>
       <c r="X522">
         <v>77</v>
       </c>
@@ -93735,6 +96467,9 @@
       <c r="J523" s="12">
         <v>293138</v>
       </c>
+      <c r="R523" t="s">
+        <v>2484</v>
+      </c>
       <c r="X523">
         <v>62</v>
       </c>
@@ -93782,6 +96517,24 @@
       <c r="J524" s="12">
         <v>509136</v>
       </c>
+      <c r="K524" t="s">
+        <v>53</v>
+      </c>
+      <c r="L524" t="s">
+        <v>32</v>
+      </c>
+      <c r="S524" s="3">
+        <v>39630</v>
+      </c>
+      <c r="U524" t="s">
+        <v>40</v>
+      </c>
+      <c r="V524" t="s">
+        <v>157</v>
+      </c>
+      <c r="W524" t="s">
+        <v>157</v>
+      </c>
       <c r="X524">
         <v>27</v>
       </c>
@@ -93829,6 +96582,9 @@
       <c r="J525" s="12">
         <v>682611</v>
       </c>
+      <c r="R525" t="s">
+        <v>2484</v>
+      </c>
       <c r="X525">
         <v>69</v>
       </c>
@@ -93876,6 +96632,27 @@
       <c r="J526" s="12">
         <v>154372</v>
       </c>
+      <c r="K526" t="s">
+        <v>30</v>
+      </c>
+      <c r="L526" t="s">
+        <v>32</v>
+      </c>
+      <c r="S526" s="3">
+        <v>37561</v>
+      </c>
+      <c r="T526" s="3">
+        <v>37562</v>
+      </c>
+      <c r="U526" t="s">
+        <v>32</v>
+      </c>
+      <c r="V526" t="s">
+        <v>157</v>
+      </c>
+      <c r="W526" t="s">
+        <v>157</v>
+      </c>
       <c r="X526">
         <v>25</v>
       </c>
@@ -93923,6 +96700,30 @@
       <c r="J527" s="12">
         <v>249222</v>
       </c>
+      <c r="K527" t="s">
+        <v>30</v>
+      </c>
+      <c r="L527" t="s">
+        <v>2594</v>
+      </c>
+      <c r="R527" t="s">
+        <v>2596</v>
+      </c>
+      <c r="S527" s="3">
+        <v>40909</v>
+      </c>
+      <c r="T527" s="3">
+        <v>40917</v>
+      </c>
+      <c r="U527" t="s">
+        <v>2593</v>
+      </c>
+      <c r="V527" t="s">
+        <v>60</v>
+      </c>
+      <c r="W527" t="s">
+        <v>34</v>
+      </c>
       <c r="X527">
         <v>77</v>
       </c>
@@ -93940,7 +96741,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="S1 S4:S5 S7 S9:S12 S15:S1048576">
+  <conditionalFormatting sqref="S1 S4:S5 S7 S9:S12 S514:S1048576 S15:S229 S231:S512">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>"Q:Q"</formula>
     </cfRule>
@@ -93954,30 +96755,259 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{273F87BA-0AD7-46D4-8854-FB1FAD0112B3}">
+  <dimension ref="B1:F32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="B1" s="13" t="s">
+        <v>2597</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" t="s">
+        <v>2598</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2599</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2601</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" t="s">
+        <v>2602</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2603</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2604</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" t="s">
+        <v>2605</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2606</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="13" t="s">
+        <v>2607</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>2608</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" t="s">
+        <v>2609</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2610</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2611</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2612</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2613</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" t="s">
+        <v>2440</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2610</v>
+      </c>
+      <c r="D11" s="15">
+        <v>12871</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2614</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2615</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" t="s">
+        <v>2616</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2617</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2618</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2619</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" t="s">
+        <v>2439</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2613</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" t="s">
+        <v>2437</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2617</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2566</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="13" t="s">
+        <v>2620</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" t="s">
+        <v>2621</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2622</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" t="s">
+        <v>2440</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2623</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" t="s">
+        <v>2616</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2625</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>2626</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" t="s">
+        <v>2439</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2627</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" t="s">
+        <v>2437</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2628</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>2629</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="13" t="s">
+        <v>2630</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" t="s">
+        <v>2631</v>
+      </c>
+      <c r="D26">
+        <v>36721</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="D27">
+        <v>455593</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="D28">
+        <v>300055956</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" t="s">
+        <v>2632</v>
+      </c>
+      <c r="D30">
+        <v>741529</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="D31">
+        <v>300938</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="D32">
+        <v>300375656</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D9" r:id="rId1" xr:uid="{7AB24406-6A50-426E-9C92-38D22BE6910D}"/>
+    <hyperlink ref="D19" r:id="rId2" xr:uid="{639B6319-109E-4D29-8CBC-5B97E3AC6A46}"/>
+    <hyperlink ref="D20" r:id="rId3" xr:uid="{D5E362B5-1840-4DC8-AB51-251B88347F8D}"/>
+    <hyperlink ref="D22" r:id="rId4" xr:uid="{FC948EFD-D4BE-4D60-9005-EEC84A28C642}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="7e17ebe2-ea76-4bcf-af9b-ad4b73b55788">
-      <UserInfo>
-        <DisplayName>Hefti Eva</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101007C90313681D0404CA6EEE81DD4C9F0C9" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="4a206f6187e2cad7d4e982dfa28e7d04">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7c5cb915-ffee-4a76-a520-e563b15a0b98" xmlns:ns3="7e17ebe2-ea76-4bcf-af9b-ad4b73b55788" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f164e3b8715a45d23ef57d38676d8631" ns2:_="" ns3:_="">
     <xsd:import namespace="7c5cb915-ffee-4a76-a520-e563b15a0b98"/>
@@ -94148,16 +97178,39 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="7e17ebe2-ea76-4bcf-af9b-ad4b73b55788">
+      <UserInfo>
+        <DisplayName>Hefti Eva</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1D568A2-F3AE-4384-B390-76487FDA7C7C}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D72925E-D78A-4D5C-8862-2F8D4DFFE495}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D540F89-8CFF-4EE3-BB1C-505451778312}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1D568A2-F3AE-4384-B390-76487FDA7C7C}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>